<commit_message>
Add new APIs: - Update user info - Search users by name - Search articles
</commit_message>
<xml_diff>
--- a/doc/detail_design/api/MCS_Web_API_Specification.xlsx
+++ b/doc/detail_design/api/MCS_Web_API_Specification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="-19140" windowWidth="27480" windowHeight="14520" tabRatio="957" activeTab="5"/>
+    <workbookView xWindow="5620" yWindow="-19140" windowWidth="27480" windowHeight="14520" tabRatio="957" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="23" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="350">
   <si>
     <t>Description</t>
   </si>
@@ -693,9 +693,6 @@
     <t>Get some user's public info.</t>
   </si>
   <si>
-    <t>POST: /users (with the variables in the entity-body)</t>
-  </si>
-  <si>
     <t>Sample URI</t>
   </si>
   <si>
@@ -729,12 +726,6 @@
     <t>Create new article for current user.</t>
   </si>
   <si>
-    <t>PUT /auth/logout</t>
-  </si>
-  <si>
-    <t>POST /auth/{username}/login</t>
-  </si>
-  <si>
     <t>Get all articles for current user.</t>
   </si>
   <si>
@@ -1069,12 +1060,6 @@
   </si>
   <si>
     <t>Search users by name</t>
-  </si>
-  <si>
-    <t>GET /v1/users/list/vutm</t>
-  </si>
-  <si>
-    <t>Search all users by first name or last name.</t>
   </si>
   <si>
     <t>/v1/users/login</t>
@@ -1093,12 +1078,36 @@
       <t>response</t>
     </r>
   </si>
+  <si>
+    <t>PUT /v1/users</t>
+  </si>
+  <si>
+    <t>Update user info (not include password).</t>
+  </si>
+  <si>
+    <t>Search users by some conditions.</t>
+  </si>
+  <si>
+    <t>GET /v1/users?name=xxx&amp;email=zzz</t>
+  </si>
+  <si>
+    <t>GET /v1/articles?keyword=xxx</t>
+  </si>
+  <si>
+    <t>Search articles that title or content matched some keyword.</t>
+  </si>
+  <si>
+    <t>Update user info</t>
+  </si>
+  <si>
+    <t>Search articles</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1296,6 +1305,11 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1542,7 +1556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="398">
+  <cellStyleXfs count="400">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1941,8 +1955,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2260,44 +2276,48 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="243" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2329,16 +2349,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2366,21 +2376,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -2393,51 +2388,72 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2473,21 +2489,19 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2503,8 +2517,28 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="398">
+  <cellStyles count="400">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2827,6 +2861,8 @@
     <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4450,299 +4486,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="43" customFormat="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="171" t="s">
+      <c r="B1" s="138"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="172"/>
-      <c r="K1" s="176" t="s">
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="177"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="158" t="s">
+      <c r="L1" s="143"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="145" t="s">
         <v>197</v>
       </c>
-      <c r="O1" s="159"/>
-      <c r="P1" s="159"/>
-      <c r="Q1" s="159"/>
-      <c r="R1" s="159"/>
-      <c r="S1" s="159"/>
-      <c r="T1" s="159"/>
-      <c r="U1" s="160"/>
-      <c r="V1" s="179" t="s">
+      <c r="O1" s="146"/>
+      <c r="P1" s="146"/>
+      <c r="Q1" s="146"/>
+      <c r="R1" s="146"/>
+      <c r="S1" s="146"/>
+      <c r="T1" s="146"/>
+      <c r="U1" s="147"/>
+      <c r="V1" s="148" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="181"/>
+      <c r="W1" s="149"/>
+      <c r="X1" s="149"/>
+      <c r="Y1" s="149"/>
+      <c r="Z1" s="149"/>
+      <c r="AA1" s="149"/>
+      <c r="AB1" s="149"/>
+      <c r="AC1" s="149"/>
+      <c r="AD1" s="150"/>
     </row>
     <row r="2" spans="1:30" s="43" customFormat="1">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171" t="s">
+      <c r="B2" s="138"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="140" t="s">
         <v>200</v>
       </c>
-      <c r="E2" s="172"/>
-      <c r="F2" s="172"/>
-      <c r="G2" s="172"/>
-      <c r="H2" s="172"/>
-      <c r="I2" s="172"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="153" t="s">
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="154"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="173" t="s">
+      <c r="L2" s="155"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="166" t="s">
         <v>202</v>
       </c>
-      <c r="O2" s="174"/>
-      <c r="P2" s="174"/>
-      <c r="Q2" s="174"/>
-      <c r="R2" s="174"/>
-      <c r="S2" s="174"/>
-      <c r="T2" s="174"/>
-      <c r="U2" s="175"/>
-      <c r="V2" s="150" t="s">
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
+      <c r="Q2" s="167"/>
+      <c r="R2" s="167"/>
+      <c r="S2" s="167"/>
+      <c r="T2" s="167"/>
+      <c r="U2" s="168"/>
+      <c r="V2" s="151" t="s">
         <v>204</v>
       </c>
-      <c r="W2" s="151"/>
-      <c r="X2" s="152"/>
-      <c r="Y2" s="150" t="s">
+      <c r="W2" s="152"/>
+      <c r="X2" s="153"/>
+      <c r="Y2" s="151" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="151"/>
-      <c r="AA2" s="152"/>
-      <c r="AB2" s="150" t="s">
+      <c r="Z2" s="152"/>
+      <c r="AA2" s="153"/>
+      <c r="AB2" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="AC2" s="151"/>
-      <c r="AD2" s="152"/>
+      <c r="AC2" s="152"/>
+      <c r="AD2" s="153"/>
     </row>
     <row r="3" spans="1:30" s="43" customFormat="1">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="154"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="156" t="s">
+      <c r="B3" s="155"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="157" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="153" t="s">
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="154" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="154"/>
-      <c r="M3" s="155"/>
-      <c r="N3" s="158" t="s">
+      <c r="L3" s="155"/>
+      <c r="M3" s="156"/>
+      <c r="N3" s="145" t="s">
         <v>203</v>
       </c>
-      <c r="O3" s="159"/>
-      <c r="P3" s="159"/>
-      <c r="Q3" s="159"/>
-      <c r="R3" s="159"/>
-      <c r="S3" s="159"/>
-      <c r="T3" s="159"/>
-      <c r="U3" s="160"/>
-      <c r="V3" s="161" t="s">
+      <c r="O3" s="146"/>
+      <c r="P3" s="146"/>
+      <c r="Q3" s="146"/>
+      <c r="R3" s="146"/>
+      <c r="S3" s="146"/>
+      <c r="T3" s="146"/>
+      <c r="U3" s="147"/>
+      <c r="V3" s="159" t="s">
         <v>205</v>
       </c>
-      <c r="W3" s="162"/>
-      <c r="X3" s="163"/>
-      <c r="Y3" s="164"/>
-      <c r="Z3" s="165"/>
-      <c r="AA3" s="166"/>
-      <c r="AB3" s="167"/>
-      <c r="AC3" s="165"/>
-      <c r="AD3" s="166"/>
+      <c r="W3" s="160"/>
+      <c r="X3" s="161"/>
+      <c r="Y3" s="162"/>
+      <c r="Z3" s="163"/>
+      <c r="AA3" s="164"/>
+      <c r="AB3" s="165"/>
+      <c r="AC3" s="163"/>
+      <c r="AD3" s="164"/>
     </row>
     <row r="7" spans="1:30" ht="16" thickBot="1"/>
     <row r="8" spans="1:30" ht="16" thickBot="1">
-      <c r="B8" s="148" t="s">
+      <c r="B8" s="181" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="148" t="s">
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="148"/>
-      <c r="H8" s="148" t="s">
+      <c r="G8" s="181"/>
+      <c r="H8" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="148"/>
-      <c r="J8" s="148"/>
-      <c r="K8" s="148" t="s">
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="148"/>
-      <c r="M8" s="148"/>
-      <c r="N8" s="148"/>
-      <c r="O8" s="148"/>
-      <c r="P8" s="148"/>
-      <c r="Q8" s="148"/>
-      <c r="R8" s="148"/>
-      <c r="S8" s="148"/>
-      <c r="T8" s="148"/>
-      <c r="U8" s="148"/>
-      <c r="V8" s="148"/>
-      <c r="W8" s="148"/>
-      <c r="X8" s="148" t="s">
+      <c r="L8" s="181"/>
+      <c r="M8" s="181"/>
+      <c r="N8" s="181"/>
+      <c r="O8" s="181"/>
+      <c r="P8" s="181"/>
+      <c r="Q8" s="181"/>
+      <c r="R8" s="181"/>
+      <c r="S8" s="181"/>
+      <c r="T8" s="181"/>
+      <c r="U8" s="181"/>
+      <c r="V8" s="181"/>
+      <c r="W8" s="181"/>
+      <c r="X8" s="181" t="s">
         <v>50</v>
       </c>
-      <c r="Y8" s="148"/>
-      <c r="Z8" s="148"/>
-      <c r="AA8" s="148"/>
-      <c r="AB8" s="148"/>
-      <c r="AC8" s="148"/>
+      <c r="Y8" s="181"/>
+      <c r="Z8" s="181"/>
+      <c r="AA8" s="181"/>
+      <c r="AB8" s="181"/>
+      <c r="AC8" s="181"/>
     </row>
     <row r="9" spans="1:30">
-      <c r="B9" s="149" t="s">
+      <c r="B9" s="169" t="s">
         <v>199</v>
       </c>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="139"/>
-      <c r="F9" s="140" t="s">
+      <c r="C9" s="170"/>
+      <c r="D9" s="170"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="172" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="141"/>
-      <c r="H9" s="137"/>
-      <c r="I9" s="138"/>
-      <c r="J9" s="139"/>
-      <c r="K9" s="142"/>
-      <c r="L9" s="143"/>
-      <c r="M9" s="143"/>
-      <c r="N9" s="143"/>
-      <c r="O9" s="143"/>
-      <c r="P9" s="143"/>
-      <c r="Q9" s="143"/>
-      <c r="R9" s="143"/>
-      <c r="S9" s="143"/>
-      <c r="T9" s="143"/>
-      <c r="U9" s="143"/>
-      <c r="V9" s="143"/>
-      <c r="W9" s="144"/>
-      <c r="X9" s="145"/>
-      <c r="Y9" s="146"/>
-      <c r="Z9" s="146"/>
-      <c r="AA9" s="146"/>
-      <c r="AB9" s="146"/>
-      <c r="AC9" s="147"/>
+      <c r="G9" s="173"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="171"/>
+      <c r="K9" s="175"/>
+      <c r="L9" s="176"/>
+      <c r="M9" s="176"/>
+      <c r="N9" s="176"/>
+      <c r="O9" s="176"/>
+      <c r="P9" s="176"/>
+      <c r="Q9" s="176"/>
+      <c r="R9" s="176"/>
+      <c r="S9" s="176"/>
+      <c r="T9" s="176"/>
+      <c r="U9" s="176"/>
+      <c r="V9" s="176"/>
+      <c r="W9" s="177"/>
+      <c r="X9" s="178"/>
+      <c r="Y9" s="179"/>
+      <c r="Z9" s="179"/>
+      <c r="AA9" s="179"/>
+      <c r="AB9" s="179"/>
+      <c r="AC9" s="180"/>
     </row>
     <row r="10" spans="1:30">
-      <c r="B10" s="137"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="141"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="138"/>
-      <c r="J10" s="139"/>
-      <c r="K10" s="142"/>
-      <c r="L10" s="143"/>
-      <c r="M10" s="143"/>
-      <c r="N10" s="143"/>
-      <c r="O10" s="143"/>
-      <c r="P10" s="143"/>
-      <c r="Q10" s="143"/>
-      <c r="R10" s="143"/>
-      <c r="S10" s="143"/>
-      <c r="T10" s="143"/>
-      <c r="U10" s="143"/>
-      <c r="V10" s="143"/>
-      <c r="W10" s="144"/>
-      <c r="X10" s="145"/>
-      <c r="Y10" s="146"/>
-      <c r="Z10" s="146"/>
-      <c r="AA10" s="146"/>
-      <c r="AB10" s="146"/>
-      <c r="AC10" s="147"/>
+      <c r="B10" s="174"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="171"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="174"/>
+      <c r="I10" s="170"/>
+      <c r="J10" s="171"/>
+      <c r="K10" s="175"/>
+      <c r="L10" s="176"/>
+      <c r="M10" s="176"/>
+      <c r="N10" s="176"/>
+      <c r="O10" s="176"/>
+      <c r="P10" s="176"/>
+      <c r="Q10" s="176"/>
+      <c r="R10" s="176"/>
+      <c r="S10" s="176"/>
+      <c r="T10" s="176"/>
+      <c r="U10" s="176"/>
+      <c r="V10" s="176"/>
+      <c r="W10" s="177"/>
+      <c r="X10" s="178"/>
+      <c r="Y10" s="179"/>
+      <c r="Z10" s="179"/>
+      <c r="AA10" s="179"/>
+      <c r="AB10" s="179"/>
+      <c r="AC10" s="180"/>
     </row>
     <row r="11" spans="1:30">
-      <c r="B11" s="137"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="141"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="138"/>
-      <c r="J11" s="139"/>
-      <c r="K11" s="142"/>
-      <c r="L11" s="143"/>
-      <c r="M11" s="143"/>
-      <c r="N11" s="143"/>
-      <c r="O11" s="143"/>
-      <c r="P11" s="143"/>
-      <c r="Q11" s="143"/>
-      <c r="R11" s="143"/>
-      <c r="S11" s="143"/>
-      <c r="T11" s="143"/>
-      <c r="U11" s="143"/>
-      <c r="V11" s="143"/>
-      <c r="W11" s="144"/>
-      <c r="X11" s="145"/>
-      <c r="Y11" s="146"/>
-      <c r="Z11" s="146"/>
-      <c r="AA11" s="146"/>
-      <c r="AB11" s="146"/>
-      <c r="AC11" s="147"/>
+      <c r="B11" s="174"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="170"/>
+      <c r="E11" s="171"/>
+      <c r="F11" s="172"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="170"/>
+      <c r="J11" s="171"/>
+      <c r="K11" s="175"/>
+      <c r="L11" s="176"/>
+      <c r="M11" s="176"/>
+      <c r="N11" s="176"/>
+      <c r="O11" s="176"/>
+      <c r="P11" s="176"/>
+      <c r="Q11" s="176"/>
+      <c r="R11" s="176"/>
+      <c r="S11" s="176"/>
+      <c r="T11" s="176"/>
+      <c r="U11" s="176"/>
+      <c r="V11" s="176"/>
+      <c r="W11" s="177"/>
+      <c r="X11" s="178"/>
+      <c r="Y11" s="179"/>
+      <c r="Z11" s="179"/>
+      <c r="AA11" s="179"/>
+      <c r="AB11" s="179"/>
+      <c r="AC11" s="180"/>
     </row>
     <row r="12" spans="1:30">
-      <c r="B12" s="137"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="141"/>
-      <c r="H12" s="137"/>
-      <c r="I12" s="138"/>
-      <c r="J12" s="139"/>
-      <c r="K12" s="142"/>
-      <c r="L12" s="143"/>
-      <c r="M12" s="143"/>
-      <c r="N12" s="143"/>
-      <c r="O12" s="143"/>
-      <c r="P12" s="143"/>
-      <c r="Q12" s="143"/>
-      <c r="R12" s="143"/>
-      <c r="S12" s="143"/>
-      <c r="T12" s="143"/>
-      <c r="U12" s="143"/>
-      <c r="V12" s="143"/>
-      <c r="W12" s="144"/>
-      <c r="X12" s="145"/>
-      <c r="Y12" s="146"/>
-      <c r="Z12" s="146"/>
-      <c r="AA12" s="146"/>
-      <c r="AB12" s="146"/>
-      <c r="AC12" s="147"/>
+      <c r="B12" s="174"/>
+      <c r="C12" s="170"/>
+      <c r="D12" s="170"/>
+      <c r="E12" s="171"/>
+      <c r="F12" s="172"/>
+      <c r="G12" s="173"/>
+      <c r="H12" s="174"/>
+      <c r="I12" s="170"/>
+      <c r="J12" s="171"/>
+      <c r="K12" s="175"/>
+      <c r="L12" s="176"/>
+      <c r="M12" s="176"/>
+      <c r="N12" s="176"/>
+      <c r="O12" s="176"/>
+      <c r="P12" s="176"/>
+      <c r="Q12" s="176"/>
+      <c r="R12" s="176"/>
+      <c r="S12" s="176"/>
+      <c r="T12" s="176"/>
+      <c r="U12" s="176"/>
+      <c r="V12" s="176"/>
+      <c r="W12" s="177"/>
+      <c r="X12" s="178"/>
+      <c r="Y12" s="179"/>
+      <c r="Z12" s="179"/>
+      <c r="AA12" s="179"/>
+      <c r="AB12" s="179"/>
+      <c r="AC12" s="180"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1"/>
     <row r="14" spans="1:30" ht="18" customHeight="1"/>
@@ -4772,11 +4808,31 @@
     <row r="38" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:W12"/>
+    <mergeCell ref="X12:AC12"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:W10"/>
+    <mergeCell ref="X10:AC10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:W11"/>
+    <mergeCell ref="X11:AC11"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:W8"/>
+    <mergeCell ref="X8:AC8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:W9"/>
+    <mergeCell ref="X9:AC9"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="A3:C3"/>
@@ -4791,31 +4847,11 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:U2"/>
     <mergeCell ref="V2:X2"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:W9"/>
-    <mergeCell ref="X9:AC9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:W8"/>
-    <mergeCell ref="X8:AC8"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:W11"/>
-    <mergeCell ref="X11:AC11"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:W10"/>
-    <mergeCell ref="X10:AC10"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:W12"/>
-    <mergeCell ref="X12:AC12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AD1"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5922,15 +5958,15 @@
       <c r="C4" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="187" t="s">
+      <c r="D4" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="187"/>
-      <c r="F4" s="187" t="s">
+      <c r="E4" s="190"/>
+      <c r="F4" s="190" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="187"/>
-      <c r="H4" s="187"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
       <c r="I4" s="125"/>
       <c r="J4" s="122"/>
       <c r="K4" s="122"/>
@@ -5945,13 +5981,13 @@
       <c r="C5" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="182" t="s">
+      <c r="D5" s="187" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="182"/>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183"/>
-      <c r="H5" s="183"/>
+      <c r="E5" s="187"/>
+      <c r="F5" s="189"/>
+      <c r="G5" s="189"/>
+      <c r="H5" s="189"/>
       <c r="I5" s="125"/>
       <c r="J5" s="125"/>
     </row>
@@ -6008,15 +6044,15 @@
       <c r="C9" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="187" t="s">
+      <c r="D9" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="187"/>
-      <c r="F9" s="187" t="s">
+      <c r="E9" s="190"/>
+      <c r="F9" s="190" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="190"/>
     </row>
     <row r="10" spans="2:14" ht="20" customHeight="1">
       <c r="B10" s="126">
@@ -6025,15 +6061,15 @@
       <c r="C10" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="182" t="s">
+      <c r="D10" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="182"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="183"/>
-      <c r="H10" s="183"/>
+      <c r="E10" s="187"/>
+      <c r="F10" s="189"/>
+      <c r="G10" s="189"/>
+      <c r="H10" s="189"/>
       <c r="I10" s="125" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="J10" s="125"/>
     </row>
@@ -6044,13 +6080,13 @@
       <c r="C11" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="182" t="s">
+      <c r="D11" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="182"/>
-      <c r="F11" s="183"/>
-      <c r="G11" s="183"/>
-      <c r="H11" s="183"/>
+      <c r="E11" s="187"/>
+      <c r="F11" s="189"/>
+      <c r="G11" s="189"/>
+      <c r="H11" s="189"/>
       <c r="I11" s="125"/>
       <c r="J11" s="125"/>
     </row>
@@ -6061,13 +6097,13 @@
       <c r="C12" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="182" t="s">
+      <c r="D12" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="182"/>
-      <c r="F12" s="183"/>
-      <c r="G12" s="183"/>
-      <c r="H12" s="183"/>
+      <c r="E12" s="187"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="189"/>
+      <c r="H12" s="189"/>
       <c r="I12" s="125"/>
       <c r="J12" s="125"/>
     </row>
@@ -6078,13 +6114,13 @@
       <c r="C13" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="182" t="s">
+      <c r="D13" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="182"/>
-      <c r="F13" s="183"/>
-      <c r="G13" s="183"/>
-      <c r="H13" s="183"/>
+      <c r="E13" s="187"/>
+      <c r="F13" s="189"/>
+      <c r="G13" s="189"/>
+      <c r="H13" s="189"/>
       <c r="I13" s="125"/>
       <c r="J13" s="125"/>
     </row>
@@ -6095,13 +6131,13 @@
       <c r="C14" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="182" t="s">
+      <c r="D14" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="182"/>
-      <c r="F14" s="183"/>
-      <c r="G14" s="183"/>
-      <c r="H14" s="183"/>
+      <c r="E14" s="187"/>
+      <c r="F14" s="189"/>
+      <c r="G14" s="189"/>
+      <c r="H14" s="189"/>
       <c r="I14" s="125"/>
       <c r="J14" s="125"/>
     </row>
@@ -6112,13 +6148,13 @@
       <c r="C15" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="182" t="s">
+      <c r="D15" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="182"/>
-      <c r="F15" s="183"/>
-      <c r="G15" s="183"/>
-      <c r="H15" s="183"/>
+      <c r="E15" s="187"/>
+      <c r="F15" s="189"/>
+      <c r="G15" s="189"/>
+      <c r="H15" s="189"/>
       <c r="I15" s="125"/>
       <c r="J15" s="125"/>
     </row>
@@ -6137,15 +6173,15 @@
       <c r="C18" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="187" t="s">
+      <c r="D18" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="187"/>
-      <c r="F18" s="187" t="s">
+      <c r="E18" s="190"/>
+      <c r="F18" s="190" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="187"/>
-      <c r="H18" s="187"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="190"/>
     </row>
     <row r="19" spans="2:10" ht="20" customHeight="1">
       <c r="B19" s="126">
@@ -6154,10 +6190,10 @@
       <c r="C19" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="182" t="s">
+      <c r="D19" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="182"/>
+      <c r="E19" s="187"/>
       <c r="F19" s="184"/>
       <c r="G19" s="185"/>
       <c r="H19" s="186"/>
@@ -6171,10 +6207,10 @@
       <c r="C20" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="182" t="s">
+      <c r="D20" s="187" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="182"/>
+      <c r="E20" s="187"/>
       <c r="F20" s="184"/>
       <c r="G20" s="185"/>
       <c r="H20" s="186"/>
@@ -6188,10 +6224,10 @@
       <c r="C21" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="182" t="s">
+      <c r="D21" s="187" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="182"/>
+      <c r="E21" s="187"/>
       <c r="F21" s="184"/>
       <c r="G21" s="185"/>
       <c r="H21" s="186"/>
@@ -6205,10 +6241,10 @@
       <c r="C22" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="182" t="s">
+      <c r="D22" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="182"/>
+      <c r="E22" s="187"/>
       <c r="F22" s="184"/>
       <c r="G22" s="185"/>
       <c r="H22" s="186"/>
@@ -6222,10 +6258,10 @@
       <c r="C23" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="182" t="s">
+      <c r="D23" s="187" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="182"/>
+      <c r="E23" s="187"/>
       <c r="F23" s="184"/>
       <c r="G23" s="185"/>
       <c r="H23" s="186"/>
@@ -6239,10 +6275,10 @@
       <c r="C24" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="182" t="s">
+      <c r="D24" s="187" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="182"/>
+      <c r="E24" s="187"/>
       <c r="F24" s="184"/>
       <c r="G24" s="185"/>
       <c r="H24" s="186"/>
@@ -6264,15 +6300,15 @@
       <c r="C27" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="187" t="s">
+      <c r="D27" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="187"/>
-      <c r="F27" s="187" t="s">
+      <c r="E27" s="190"/>
+      <c r="F27" s="190" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="187"/>
-      <c r="H27" s="187"/>
+      <c r="G27" s="190"/>
+      <c r="H27" s="190"/>
     </row>
     <row r="28" spans="2:10" ht="20" customHeight="1">
       <c r="B28" s="126">
@@ -6281,15 +6317,15 @@
       <c r="C28" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="182" t="s">
+      <c r="D28" s="187" t="s">
         <v>101</v>
       </c>
-      <c r="E28" s="182"/>
+      <c r="E28" s="187"/>
       <c r="F28" s="184"/>
       <c r="G28" s="185"/>
       <c r="H28" s="186"/>
       <c r="I28" s="125" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J28" s="125"/>
     </row>
@@ -6300,10 +6336,10 @@
       <c r="C29" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="182" t="s">
+      <c r="D29" s="187" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="182"/>
+      <c r="E29" s="187"/>
       <c r="F29" s="184"/>
       <c r="G29" s="185"/>
       <c r="H29" s="186"/>
@@ -6317,10 +6353,10 @@
       <c r="C30" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="182" t="s">
+      <c r="D30" s="187" t="s">
         <v>103</v>
       </c>
-      <c r="E30" s="182"/>
+      <c r="E30" s="187"/>
       <c r="F30" s="184"/>
       <c r="G30" s="185"/>
       <c r="H30" s="186"/>
@@ -6334,10 +6370,10 @@
       <c r="C31" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="182" t="s">
+      <c r="D31" s="187" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="182"/>
+      <c r="E31" s="187"/>
       <c r="F31" s="184"/>
       <c r="G31" s="185"/>
       <c r="H31" s="186"/>
@@ -6351,10 +6387,10 @@
       <c r="C32" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="182" t="s">
+      <c r="D32" s="187" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="182"/>
+      <c r="E32" s="187"/>
       <c r="F32" s="184"/>
       <c r="G32" s="185"/>
       <c r="H32" s="186"/>
@@ -6368,10 +6404,10 @@
       <c r="C33" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="182" t="s">
+      <c r="D33" s="187" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="182"/>
+      <c r="E33" s="187"/>
       <c r="F33" s="184"/>
       <c r="G33" s="185"/>
       <c r="H33" s="186"/>
@@ -6385,10 +6421,10 @@
       <c r="C34" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="182" t="s">
+      <c r="D34" s="187" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="182"/>
+      <c r="E34" s="187"/>
       <c r="F34" s="184"/>
       <c r="G34" s="185"/>
       <c r="H34" s="186"/>
@@ -6402,10 +6438,10 @@
       <c r="C35" s="127" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="182" t="s">
+      <c r="D35" s="187" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="182"/>
+      <c r="E35" s="187"/>
       <c r="F35" s="184"/>
       <c r="G35" s="185"/>
       <c r="H35" s="186"/>
@@ -6419,10 +6455,10 @@
       <c r="C36" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="182" t="s">
+      <c r="D36" s="187" t="s">
         <v>113</v>
       </c>
-      <c r="E36" s="182"/>
+      <c r="E36" s="187"/>
       <c r="F36" s="184"/>
       <c r="G36" s="185"/>
       <c r="H36" s="186"/>
@@ -6440,11 +6476,11 @@
     <row r="40" spans="2:10">
       <c r="B40" s="124"/>
       <c r="C40" s="124"/>
-      <c r="D40" s="190"/>
-      <c r="E40" s="190"/>
-      <c r="F40" s="190"/>
-      <c r="G40" s="190"/>
-      <c r="H40" s="190"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="188"/>
+      <c r="F40" s="188"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1">
       <c r="B41" s="126">
@@ -6453,10 +6489,10 @@
       <c r="C41" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="188" t="s">
+      <c r="D41" s="182" t="s">
         <v>157</v>
       </c>
-      <c r="E41" s="189"/>
+      <c r="E41" s="183"/>
       <c r="F41" s="184"/>
       <c r="G41" s="185"/>
       <c r="H41" s="186"/>
@@ -6468,10 +6504,10 @@
       <c r="C42" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="D42" s="188" t="s">
+      <c r="D42" s="182" t="s">
         <v>162</v>
       </c>
-      <c r="E42" s="189"/>
+      <c r="E42" s="183"/>
       <c r="F42" s="184"/>
       <c r="G42" s="185"/>
       <c r="H42" s="186"/>
@@ -6483,8 +6519,8 @@
       <c r="C43" s="127" t="s">
         <v>154</v>
       </c>
-      <c r="D43" s="188"/>
-      <c r="E43" s="189"/>
+      <c r="D43" s="182"/>
+      <c r="E43" s="183"/>
       <c r="F43" s="184"/>
       <c r="G43" s="185"/>
       <c r="H43" s="186"/>
@@ -6496,8 +6532,8 @@
       <c r="C44" s="127" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="188"/>
-      <c r="E44" s="189"/>
+      <c r="D44" s="182"/>
+      <c r="E44" s="183"/>
       <c r="F44" s="184"/>
       <c r="G44" s="185"/>
       <c r="H44" s="186"/>
@@ -6509,8 +6545,8 @@
       <c r="C45" s="127" t="s">
         <v>156</v>
       </c>
-      <c r="D45" s="188"/>
-      <c r="E45" s="189"/>
+      <c r="D45" s="182"/>
+      <c r="E45" s="183"/>
       <c r="F45" s="184"/>
       <c r="G45" s="185"/>
       <c r="H45" s="186"/>
@@ -6526,11 +6562,11 @@
     <row r="49" spans="2:8">
       <c r="B49" s="124"/>
       <c r="C49" s="124"/>
-      <c r="D49" s="190"/>
-      <c r="E49" s="190"/>
-      <c r="F49" s="190"/>
-      <c r="G49" s="190"/>
-      <c r="H49" s="190"/>
+      <c r="D49" s="188"/>
+      <c r="E49" s="188"/>
+      <c r="F49" s="188"/>
+      <c r="G49" s="188"/>
+      <c r="H49" s="188"/>
     </row>
     <row r="50" spans="2:8" ht="20" customHeight="1">
       <c r="B50" s="126">
@@ -6539,10 +6575,10 @@
       <c r="C50" s="127" t="s">
         <v>122</v>
       </c>
-      <c r="D50" s="182" t="s">
+      <c r="D50" s="187" t="s">
         <v>121</v>
       </c>
-      <c r="E50" s="182"/>
+      <c r="E50" s="187"/>
       <c r="F50" s="184"/>
       <c r="G50" s="185"/>
       <c r="H50" s="186"/>
@@ -6554,10 +6590,10 @@
       <c r="C51" s="127" t="s">
         <v>123</v>
       </c>
-      <c r="D51" s="182" t="s">
+      <c r="D51" s="187" t="s">
         <v>129</v>
       </c>
-      <c r="E51" s="182"/>
+      <c r="E51" s="187"/>
       <c r="F51" s="184"/>
       <c r="G51" s="185"/>
       <c r="H51" s="186"/>
@@ -6569,10 +6605,10 @@
       <c r="C52" s="127" t="s">
         <v>124</v>
       </c>
-      <c r="D52" s="182" t="s">
+      <c r="D52" s="187" t="s">
         <v>130</v>
       </c>
-      <c r="E52" s="182"/>
+      <c r="E52" s="187"/>
       <c r="F52" s="184"/>
       <c r="G52" s="185"/>
       <c r="H52" s="186"/>
@@ -6584,10 +6620,10 @@
       <c r="C53" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="D53" s="182" t="s">
+      <c r="D53" s="187" t="s">
         <v>131</v>
       </c>
-      <c r="E53" s="182"/>
+      <c r="E53" s="187"/>
       <c r="F53" s="184"/>
       <c r="G53" s="185"/>
       <c r="H53" s="186"/>
@@ -6599,10 +6635,10 @@
       <c r="C54" s="127" t="s">
         <v>126</v>
       </c>
-      <c r="D54" s="182" t="s">
+      <c r="D54" s="187" t="s">
         <v>132</v>
       </c>
-      <c r="E54" s="182"/>
+      <c r="E54" s="187"/>
       <c r="F54" s="184"/>
       <c r="G54" s="185"/>
       <c r="H54" s="186"/>
@@ -6614,10 +6650,10 @@
       <c r="C55" s="127" t="s">
         <v>127</v>
       </c>
-      <c r="D55" s="182" t="s">
+      <c r="D55" s="187" t="s">
         <v>133</v>
       </c>
-      <c r="E55" s="182"/>
+      <c r="E55" s="187"/>
       <c r="F55" s="184"/>
       <c r="G55" s="185"/>
       <c r="H55" s="186"/>
@@ -6629,10 +6665,10 @@
       <c r="C56" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="D56" s="182" t="s">
+      <c r="D56" s="187" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="182"/>
+      <c r="E56" s="187"/>
       <c r="F56" s="184"/>
       <c r="G56" s="185"/>
       <c r="H56" s="186"/>
@@ -6648,11 +6684,11 @@
     <row r="60" spans="2:8">
       <c r="B60" s="124"/>
       <c r="C60" s="124"/>
-      <c r="D60" s="190"/>
-      <c r="E60" s="190"/>
-      <c r="F60" s="190"/>
-      <c r="G60" s="190"/>
-      <c r="H60" s="190"/>
+      <c r="D60" s="188"/>
+      <c r="E60" s="188"/>
+      <c r="F60" s="188"/>
+      <c r="G60" s="188"/>
+      <c r="H60" s="188"/>
     </row>
     <row r="61" spans="2:8" ht="15" customHeight="1">
       <c r="B61" s="126">
@@ -6661,10 +6697,10 @@
       <c r="C61" s="127" t="s">
         <v>136</v>
       </c>
-      <c r="D61" s="188" t="s">
+      <c r="D61" s="182" t="s">
         <v>141</v>
       </c>
-      <c r="E61" s="189"/>
+      <c r="E61" s="183"/>
       <c r="F61" s="184"/>
       <c r="G61" s="185"/>
       <c r="H61" s="186"/>
@@ -6676,10 +6712,10 @@
       <c r="C62" s="127" t="s">
         <v>137</v>
       </c>
-      <c r="D62" s="188" t="s">
+      <c r="D62" s="182" t="s">
         <v>142</v>
       </c>
-      <c r="E62" s="189"/>
+      <c r="E62" s="183"/>
       <c r="F62" s="184"/>
       <c r="G62" s="185"/>
       <c r="H62" s="186"/>
@@ -6691,10 +6727,10 @@
       <c r="C63" s="127" t="s">
         <v>138</v>
       </c>
-      <c r="D63" s="188" t="s">
+      <c r="D63" s="182" t="s">
         <v>143</v>
       </c>
-      <c r="E63" s="189"/>
+      <c r="E63" s="183"/>
       <c r="F63" s="184"/>
       <c r="G63" s="185"/>
       <c r="H63" s="186"/>
@@ -6706,10 +6742,10 @@
       <c r="C64" s="127" t="s">
         <v>139</v>
       </c>
-      <c r="D64" s="188" t="s">
+      <c r="D64" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="E64" s="189"/>
+      <c r="E64" s="183"/>
       <c r="F64" s="184"/>
       <c r="G64" s="185"/>
       <c r="H64" s="186"/>
@@ -6721,32 +6757,72 @@
       <c r="C65" s="127" t="s">
         <v>140</v>
       </c>
-      <c r="D65" s="188"/>
-      <c r="E65" s="189"/>
+      <c r="D65" s="182"/>
+      <c r="E65" s="183"/>
       <c r="F65" s="184"/>
       <c r="G65" s="185"/>
       <c r="H65" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="92">
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:H14"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="F36:H36"/>
     <mergeCell ref="D51:E51"/>
@@ -6763,64 +6839,24 @@
     <mergeCell ref="F43:H43"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="F44:H44"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:H55"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6835,10 +6871,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N30"/>
+  <dimension ref="B1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6849,8 +6885,8 @@
     <col min="4" max="4" width="11.5" style="36" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="36" customWidth="1"/>
     <col min="6" max="6" width="48.6640625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="43.5" style="36" customWidth="1"/>
-    <col min="8" max="8" width="51.83203125" style="36" customWidth="1"/>
+    <col min="7" max="7" width="62.33203125" style="36" customWidth="1"/>
+    <col min="8" max="8" width="62.83203125" style="36" customWidth="1"/>
     <col min="9" max="9" width="57.5" style="36" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="36"/>
   </cols>
@@ -6899,20 +6935,17 @@
         <v>169</v>
       </c>
       <c r="D4" s="104" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E4" s="191" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F4" s="192"/>
       <c r="G4" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H4" s="104" t="s">
         <v>0</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="20" customHeight="1">
@@ -6920,7 +6953,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="106" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D5" s="193" t="s">
         <v>209</v>
@@ -6929,13 +6962,13 @@
         <v>212</v>
       </c>
       <c r="F5" s="108" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G5" s="108" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H5" s="109" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I5" s="110"/>
       <c r="J5" s="38"/>
@@ -6945,24 +6978,22 @@
         <v>2</v>
       </c>
       <c r="C6" s="106" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D6" s="194"/>
       <c r="E6" s="107" t="s">
         <v>212</v>
       </c>
       <c r="F6" s="108" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G6" s="108" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="H6" s="109" t="s">
-        <v>225</v>
-      </c>
-      <c r="I6" s="110" t="s">
-        <v>230</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="I6" s="110"/>
       <c r="J6" s="38"/>
     </row>
     <row r="7" spans="2:14" ht="20" customHeight="1">
@@ -6970,20 +7001,20 @@
         <v>3</v>
       </c>
       <c r="C7" s="106" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D7" s="194"/>
       <c r="E7" s="107" t="s">
         <v>213</v>
       </c>
       <c r="F7" s="108" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G7" s="108" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H7" s="109" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I7" s="110"/>
       <c r="J7" s="38"/>
@@ -6993,20 +7024,20 @@
         <v>4</v>
       </c>
       <c r="C8" s="106" t="s">
-        <v>243</v>
+        <v>348</v>
       </c>
       <c r="D8" s="194"/>
-      <c r="E8" s="107" t="s">
-        <v>215</v>
-      </c>
-      <c r="F8" s="108" t="s">
-        <v>262</v>
-      </c>
-      <c r="G8" s="108" t="s">
-        <v>221</v>
-      </c>
-      <c r="H8" s="109" t="s">
-        <v>216</v>
+      <c r="E8" s="216" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="G8" s="217" t="s">
+        <v>342</v>
+      </c>
+      <c r="H8" s="218" t="s">
+        <v>343</v>
       </c>
       <c r="I8" s="110"/>
       <c r="J8" s="38"/>
@@ -7016,20 +7047,20 @@
         <v>5</v>
       </c>
       <c r="C9" s="106" t="s">
-        <v>342</v>
+        <v>240</v>
       </c>
       <c r="D9" s="194"/>
       <c r="E9" s="107" t="s">
         <v>215</v>
       </c>
       <c r="F9" s="108" t="s">
-        <v>341</v>
+        <v>259</v>
       </c>
       <c r="G9" s="108" t="s">
-        <v>343</v>
+        <v>220</v>
       </c>
       <c r="H9" s="109" t="s">
-        <v>344</v>
+        <v>216</v>
       </c>
       <c r="I9" s="110"/>
       <c r="J9" s="38"/>
@@ -7039,47 +7070,43 @@
         <v>6</v>
       </c>
       <c r="C10" s="106" t="s">
-        <v>244</v>
-      </c>
-      <c r="D10" s="195"/>
-      <c r="E10" s="107" t="s">
-        <v>213</v>
-      </c>
-      <c r="F10" s="108" t="s">
-        <v>263</v>
-      </c>
-      <c r="G10" s="108" t="s">
-        <v>286</v>
-      </c>
-      <c r="H10" s="109" t="s">
-        <v>227</v>
-      </c>
-      <c r="I10" s="110" t="s">
-        <v>229</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="D10" s="194"/>
+      <c r="E10" s="216" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="217" t="s">
+        <v>338</v>
+      </c>
+      <c r="G10" s="217" t="s">
+        <v>345</v>
+      </c>
+      <c r="H10" s="218" t="s">
+        <v>344</v>
+      </c>
+      <c r="I10" s="110"/>
       <c r="J10" s="38"/>
     </row>
     <row r="11" spans="2:14" ht="20" customHeight="1">
       <c r="B11" s="105">
         <v>7</v>
       </c>
-      <c r="C11" s="111" t="s">
-        <v>248</v>
-      </c>
-      <c r="D11" s="196" t="s">
-        <v>210</v>
-      </c>
-      <c r="E11" s="112" t="s">
-        <v>215</v>
-      </c>
-      <c r="F11" s="113" t="s">
-        <v>264</v>
-      </c>
-      <c r="G11" s="113" t="s">
-        <v>222</v>
-      </c>
-      <c r="H11" s="114" t="s">
-        <v>247</v>
+      <c r="C11" s="106" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="195"/>
+      <c r="E11" s="107" t="s">
+        <v>213</v>
+      </c>
+      <c r="F11" s="108" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="108" t="s">
+        <v>283</v>
+      </c>
+      <c r="H11" s="109" t="s">
+        <v>226</v>
       </c>
       <c r="I11" s="110"/>
       <c r="J11" s="38"/>
@@ -7089,20 +7116,22 @@
         <v>8</v>
       </c>
       <c r="C12" s="111" t="s">
-        <v>246</v>
-      </c>
-      <c r="D12" s="197"/>
+        <v>245</v>
+      </c>
+      <c r="D12" s="196" t="s">
+        <v>210</v>
+      </c>
       <c r="E12" s="112" t="s">
         <v>215</v>
       </c>
       <c r="F12" s="113" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G12" s="113" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="H12" s="114" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="I12" s="110"/>
       <c r="J12" s="38"/>
@@ -7112,20 +7141,20 @@
         <v>9</v>
       </c>
       <c r="C13" s="111" t="s">
-        <v>245</v>
+        <v>349</v>
       </c>
       <c r="D13" s="197"/>
-      <c r="E13" s="112" t="s">
+      <c r="E13" s="219" t="s">
         <v>215</v>
       </c>
-      <c r="F13" s="113" t="s">
-        <v>266</v>
-      </c>
-      <c r="G13" s="113" t="s">
-        <v>272</v>
-      </c>
-      <c r="H13" s="114" t="s">
-        <v>231</v>
+      <c r="F13" s="220" t="s">
+        <v>261</v>
+      </c>
+      <c r="G13" s="220" t="s">
+        <v>346</v>
+      </c>
+      <c r="H13" s="221" t="s">
+        <v>347</v>
       </c>
       <c r="I13" s="110"/>
       <c r="J13" s="38"/>
@@ -7135,20 +7164,20 @@
         <v>10</v>
       </c>
       <c r="C14" s="111" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="D14" s="197"/>
       <c r="E14" s="112" t="s">
         <v>215</v>
       </c>
       <c r="F14" s="113" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G14" s="113" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="H14" s="114" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="I14" s="110"/>
       <c r="J14" s="38"/>
@@ -7158,17 +7187,17 @@
         <v>11</v>
       </c>
       <c r="C15" s="111" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D15" s="197"/>
       <c r="E15" s="112" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F15" s="113" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G15" s="113" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="H15" s="114" t="s">
         <v>228</v>
@@ -7181,20 +7210,20 @@
         <v>12</v>
       </c>
       <c r="C16" s="111" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D16" s="197"/>
       <c r="E16" s="112" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F16" s="113" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G16" s="113" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H16" s="114" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="I16" s="110"/>
       <c r="J16" s="38"/>
@@ -7204,20 +7233,20 @@
         <v>13</v>
       </c>
       <c r="C17" s="111" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D17" s="197"/>
       <c r="E17" s="112" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F17" s="113" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="G17" s="113" t="s">
-        <v>275</v>
+        <v>222</v>
       </c>
       <c r="H17" s="114" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I17" s="110"/>
       <c r="J17" s="38"/>
@@ -7226,23 +7255,21 @@
       <c r="B18" s="105">
         <v>14</v>
       </c>
-      <c r="C18" s="115" t="s">
-        <v>252</v>
-      </c>
-      <c r="D18" s="198" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="116" t="s">
-        <v>215</v>
-      </c>
-      <c r="F18" s="117" t="s">
-        <v>268</v>
-      </c>
-      <c r="G18" s="117" t="s">
-        <v>276</v>
-      </c>
-      <c r="H18" s="118" t="s">
-        <v>278</v>
+      <c r="C18" s="111" t="s">
+        <v>247</v>
+      </c>
+      <c r="D18" s="197"/>
+      <c r="E18" s="112" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" s="113" t="s">
+        <v>264</v>
+      </c>
+      <c r="G18" s="113" t="s">
+        <v>271</v>
+      </c>
+      <c r="H18" s="114" t="s">
+        <v>230</v>
       </c>
       <c r="I18" s="110"/>
       <c r="J18" s="38"/>
@@ -7251,21 +7278,21 @@
       <c r="B19" s="105">
         <v>15</v>
       </c>
-      <c r="C19" s="115" t="s">
-        <v>253</v>
-      </c>
-      <c r="D19" s="199"/>
-      <c r="E19" s="116" t="s">
-        <v>215</v>
-      </c>
-      <c r="F19" s="117" t="s">
-        <v>269</v>
-      </c>
-      <c r="G19" s="117" t="s">
-        <v>285</v>
-      </c>
-      <c r="H19" s="118" t="s">
-        <v>279</v>
+      <c r="C19" s="111" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" s="197"/>
+      <c r="E19" s="112" t="s">
+        <v>214</v>
+      </c>
+      <c r="F19" s="113" t="s">
+        <v>264</v>
+      </c>
+      <c r="G19" s="113" t="s">
+        <v>272</v>
+      </c>
+      <c r="H19" s="114" t="s">
+        <v>231</v>
       </c>
       <c r="I19" s="110"/>
       <c r="J19" s="38"/>
@@ -7275,20 +7302,22 @@
         <v>16</v>
       </c>
       <c r="C20" s="115" t="s">
-        <v>254</v>
-      </c>
-      <c r="D20" s="199"/>
+        <v>249</v>
+      </c>
+      <c r="D20" s="198" t="s">
+        <v>211</v>
+      </c>
       <c r="E20" s="116" t="s">
         <v>215</v>
       </c>
       <c r="F20" s="117" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G20" s="117" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H20" s="118" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="I20" s="110"/>
       <c r="J20" s="38"/>
@@ -7298,20 +7327,20 @@
         <v>17</v>
       </c>
       <c r="C21" s="115" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D21" s="199"/>
       <c r="E21" s="116" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F21" s="117" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G21" s="117" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H21" s="118" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c r="I21" s="110"/>
       <c r="J21" s="38"/>
@@ -7321,20 +7350,20 @@
         <v>18</v>
       </c>
       <c r="C22" s="115" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D22" s="199"/>
       <c r="E22" s="116" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F22" s="117" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="G22" s="117" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="H22" s="118" t="s">
-        <v>236</v>
+        <v>277</v>
       </c>
       <c r="I22" s="110"/>
       <c r="J22" s="38"/>
@@ -7344,20 +7373,20 @@
         <v>19</v>
       </c>
       <c r="C23" s="115" t="s">
-        <v>257</v>
-      </c>
-      <c r="D23" s="200"/>
+        <v>252</v>
+      </c>
+      <c r="D23" s="199"/>
       <c r="E23" s="116" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F23" s="117" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="G23" s="117" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H23" s="118" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I23" s="110"/>
       <c r="J23" s="38"/>
@@ -7366,12 +7395,22 @@
       <c r="B24" s="105">
         <v>20</v>
       </c>
-      <c r="C24" s="106"/>
-      <c r="D24" s="119"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="108"/>
-      <c r="G24" s="108"/>
-      <c r="H24" s="109"/>
+      <c r="C24" s="115" t="s">
+        <v>253</v>
+      </c>
+      <c r="D24" s="199"/>
+      <c r="E24" s="116" t="s">
+        <v>213</v>
+      </c>
+      <c r="F24" s="117" t="s">
+        <v>268</v>
+      </c>
+      <c r="G24" s="117" t="s">
+        <v>279</v>
+      </c>
+      <c r="H24" s="118" t="s">
+        <v>233</v>
+      </c>
       <c r="I24" s="110"/>
       <c r="J24" s="38"/>
     </row>
@@ -7379,12 +7418,22 @@
       <c r="B25" s="105">
         <v>21</v>
       </c>
-      <c r="C25" s="106"/>
-      <c r="D25" s="119"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="109"/>
+      <c r="C25" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="D25" s="200"/>
+      <c r="E25" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="F25" s="117" t="s">
+        <v>268</v>
+      </c>
+      <c r="G25" s="117" t="s">
+        <v>280</v>
+      </c>
+      <c r="H25" s="118" t="s">
+        <v>234</v>
+      </c>
       <c r="I25" s="110"/>
       <c r="J25" s="38"/>
     </row>
@@ -7415,44 +7464,70 @@
       <c r="J27" s="38"/>
     </row>
     <row r="28" spans="2:10" ht="20" customHeight="1">
-      <c r="B28" s="58"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="61"/>
+      <c r="B28" s="105">
+        <v>24</v>
+      </c>
+      <c r="C28" s="106"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="108"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="110"/>
       <c r="J28" s="38"/>
     </row>
     <row r="29" spans="2:10" ht="20" customHeight="1">
-      <c r="B29" s="39"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="61"/>
+      <c r="B29" s="105">
+        <v>25</v>
+      </c>
+      <c r="C29" s="106"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="108"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="110"/>
       <c r="J29" s="38"/>
     </row>
     <row r="30" spans="2:10" ht="20" customHeight="1">
-      <c r="B30" s="39"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
       <c r="I30" s="61"/>
       <c r="J30" s="38"/>
+    </row>
+    <row r="31" spans="2:10" ht="20" customHeight="1">
+      <c r="B31" s="39"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="38"/>
+    </row>
+    <row r="32" spans="2:10" ht="20" customHeight="1">
+      <c r="B32" s="39"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D5:D10"/>
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="D5:D11"/>
+    <mergeCell ref="D12:D19"/>
+    <mergeCell ref="D20:D25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7468,7 +7543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="D38" sqref="D38:E38"/>
     </sheetView>
   </sheetViews>
@@ -7511,7 +7586,7 @@
         <v>182</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -7552,13 +7627,13 @@
         <v>169</v>
       </c>
       <c r="C4" s="201" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" s="211"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
+        <v>237</v>
+      </c>
+      <c r="D4" s="209"/>
+      <c r="E4" s="209"/>
+      <c r="F4" s="209"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="209"/>
       <c r="I4" s="202"/>
       <c r="J4" s="66"/>
       <c r="K4" s="66"/>
@@ -7573,13 +7648,13 @@
         <v>170</v>
       </c>
       <c r="C5" s="201" t="s">
-        <v>224</v>
-      </c>
-      <c r="D5" s="211"/>
-      <c r="E5" s="211"/>
-      <c r="F5" s="211"/>
-      <c r="G5" s="211"/>
-      <c r="H5" s="211"/>
+        <v>223</v>
+      </c>
+      <c r="D5" s="209"/>
+      <c r="E5" s="209"/>
+      <c r="F5" s="209"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="209"/>
       <c r="I5" s="202"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
@@ -7591,10 +7666,10 @@
     <row r="6" spans="1:15" ht="20" customHeight="1">
       <c r="A6" s="66"/>
       <c r="B6" s="70" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C6" s="103" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="72"/>
@@ -7612,16 +7687,16 @@
     <row r="7" spans="1:15" ht="20" customHeight="1">
       <c r="A7" s="66"/>
       <c r="B7" s="70" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C7" s="201" t="s">
         <v>212</v>
       </c>
-      <c r="D7" s="211"/>
-      <c r="E7" s="211"/>
-      <c r="F7" s="211"/>
-      <c r="G7" s="211"/>
-      <c r="H7" s="211"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="209"/>
+      <c r="H7" s="209"/>
       <c r="I7" s="202"/>
       <c r="J7" s="66"/>
       <c r="K7" s="66"/>
@@ -7633,7 +7708,7 @@
     <row r="8" spans="1:15" ht="20" customHeight="1">
       <c r="A8" s="66"/>
       <c r="B8" s="70" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C8" s="71" t="s">
         <v>38</v>
@@ -7654,16 +7729,16 @@
     <row r="9" spans="1:15" ht="20" customHeight="1">
       <c r="A9" s="66"/>
       <c r="B9" s="70" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C9" s="201" t="s">
-        <v>336</v>
-      </c>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="211"/>
-      <c r="H9" s="211"/>
+        <v>333</v>
+      </c>
+      <c r="D9" s="209"/>
+      <c r="E9" s="209"/>
+      <c r="F9" s="209"/>
+      <c r="G9" s="209"/>
+      <c r="H9" s="209"/>
       <c r="I9" s="202"/>
       <c r="J9" s="66"/>
       <c r="K9" s="66"/>
@@ -7692,7 +7767,7 @@
     <row r="11" spans="1:15" ht="20" customHeight="1">
       <c r="A11" s="66"/>
       <c r="B11" s="74" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C11" s="74"/>
       <c r="D11" s="66"/>
@@ -7727,19 +7802,19 @@
     </row>
     <row r="13" spans="1:15" ht="20" customHeight="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="208" t="s">
+      <c r="B13" s="203" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="209"/>
-      <c r="D13" s="209"/>
-      <c r="E13" s="209"/>
-      <c r="F13" s="209"/>
-      <c r="G13" s="209"/>
-      <c r="H13" s="209"/>
-      <c r="I13" s="209"/>
-      <c r="J13" s="209"/>
-      <c r="K13" s="209"/>
-      <c r="L13" s="210"/>
+      <c r="C13" s="204"/>
+      <c r="D13" s="204"/>
+      <c r="E13" s="204"/>
+      <c r="F13" s="204"/>
+      <c r="G13" s="204"/>
+      <c r="H13" s="204"/>
+      <c r="I13" s="204"/>
+      <c r="J13" s="204"/>
+      <c r="K13" s="204"/>
+      <c r="L13" s="205"/>
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
       <c r="O13" s="66"/>
@@ -7768,11 +7843,11 @@
       <c r="I14" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="J14" s="212" t="s">
+      <c r="J14" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="212"/>
-      <c r="L14" s="212"/>
+      <c r="K14" s="210"/>
+      <c r="L14" s="210"/>
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
       <c r="O14" s="66"/>
@@ -7781,16 +7856,16 @@
       <c r="A15" s="66"/>
       <c r="B15" s="77"/>
       <c r="C15" s="78" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D15" s="79" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E15" s="80" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F15" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G15" s="80">
         <v>4</v>
@@ -7799,13 +7874,13 @@
         <v>50</v>
       </c>
       <c r="I15" s="81" t="s">
-        <v>292</v>
-      </c>
-      <c r="J15" s="213" t="s">
-        <v>293</v>
-      </c>
-      <c r="K15" s="213"/>
-      <c r="L15" s="213"/>
+        <v>289</v>
+      </c>
+      <c r="J15" s="211" t="s">
+        <v>290</v>
+      </c>
+      <c r="K15" s="211"/>
+      <c r="L15" s="211"/>
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
@@ -7814,16 +7889,16 @@
       <c r="A16" s="66"/>
       <c r="B16" s="77"/>
       <c r="C16" s="78" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D16" s="79" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E16" s="80" t="s">
         <v>183</v>
       </c>
       <c r="F16" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G16" s="80">
         <v>4</v>
@@ -7832,13 +7907,13 @@
         <v>50</v>
       </c>
       <c r="I16" s="81" t="s">
-        <v>296</v>
-      </c>
-      <c r="J16" s="213" t="s">
-        <v>297</v>
-      </c>
-      <c r="K16" s="213"/>
-      <c r="L16" s="213"/>
+        <v>293</v>
+      </c>
+      <c r="J16" s="211" t="s">
+        <v>294</v>
+      </c>
+      <c r="K16" s="211"/>
+      <c r="L16" s="211"/>
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
@@ -7847,16 +7922,16 @@
       <c r="A17" s="66"/>
       <c r="B17" s="77"/>
       <c r="C17" s="78" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D17" s="79" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E17" s="80" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F17" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G17" s="80" t="s">
         <v>180</v>
@@ -7865,10 +7940,10 @@
         <v>50</v>
       </c>
       <c r="I17" s="81" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J17" s="71" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K17" s="72"/>
       <c r="L17" s="73"/>
@@ -7880,16 +7955,16 @@
       <c r="A18" s="66"/>
       <c r="B18" s="77"/>
       <c r="C18" s="78" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D18" s="79" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E18" s="80" t="s">
         <v>184</v>
       </c>
       <c r="F18" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G18" s="80" t="s">
         <v>180</v>
@@ -7898,12 +7973,12 @@
         <v>50</v>
       </c>
       <c r="I18" s="79" t="s">
+        <v>303</v>
+      </c>
+      <c r="J18" s="201" t="s">
         <v>306</v>
       </c>
-      <c r="J18" s="201" t="s">
-        <v>309</v>
-      </c>
-      <c r="K18" s="211"/>
+      <c r="K18" s="209"/>
       <c r="L18" s="202"/>
       <c r="M18" s="66"/>
       <c r="N18" s="66"/>
@@ -7913,16 +7988,16 @@
       <c r="A19" s="66"/>
       <c r="B19" s="82"/>
       <c r="C19" s="78" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D19" s="79" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E19" s="80" t="s">
         <v>184</v>
       </c>
       <c r="F19" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G19" s="80" t="s">
         <v>180</v>
@@ -7931,12 +8006,12 @@
         <v>255</v>
       </c>
       <c r="I19" s="83" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J19" s="201" t="s">
-        <v>314</v>
-      </c>
-      <c r="K19" s="211"/>
+        <v>311</v>
+      </c>
+      <c r="K19" s="209"/>
       <c r="L19" s="202"/>
       <c r="M19" s="66"/>
       <c r="N19" s="66"/>
@@ -7962,7 +8037,7 @@
     <row r="21" spans="1:15" ht="20" customHeight="1">
       <c r="A21" s="66"/>
       <c r="B21" s="74" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="84"/>
@@ -8099,11 +8174,11 @@
     </row>
     <row r="29" spans="1:15" s="89" customFormat="1" ht="20" customHeight="1">
       <c r="A29" s="69"/>
-      <c r="B29" s="214" t="s">
-        <v>302</v>
-      </c>
-      <c r="C29" s="214"/>
-      <c r="D29" s="214"/>
+      <c r="B29" s="212" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" s="212"/>
+      <c r="D29" s="212"/>
       <c r="E29" s="87"/>
       <c r="F29" s="88"/>
       <c r="G29" s="87"/>
@@ -8118,12 +8193,12 @@
     </row>
     <row r="30" spans="1:15" s="91" customFormat="1" ht="20" customHeight="1">
       <c r="A30" s="90"/>
-      <c r="B30" s="205" t="s">
+      <c r="B30" s="206" t="s">
         <v>173</v>
       </c>
-      <c r="C30" s="206"/>
-      <c r="D30" s="206"/>
-      <c r="E30" s="207"/>
+      <c r="C30" s="207"/>
+      <c r="D30" s="207"/>
+      <c r="E30" s="208"/>
       <c r="F30" s="76" t="s">
         <v>172</v>
       </c>
@@ -8143,7 +8218,7 @@
         <v>177</v>
       </c>
       <c r="L30" s="76" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="M30" s="90"/>
       <c r="N30" s="90"/>
@@ -8184,18 +8259,18 @@
       <c r="A32" s="66"/>
       <c r="B32" s="92"/>
       <c r="C32" s="95" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D32" s="96"/>
       <c r="E32" s="94"/>
       <c r="F32" s="78" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G32" s="80" t="s">
         <v>185</v>
       </c>
       <c r="H32" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I32" s="80">
         <v>1</v>
@@ -8216,7 +8291,7 @@
       <c r="B33" s="92"/>
       <c r="C33" s="97"/>
       <c r="D33" s="201" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E33" s="202"/>
       <c r="F33" s="78" t="s">
@@ -8226,7 +8301,7 @@
         <v>181</v>
       </c>
       <c r="H33" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I33" s="80">
         <v>1</v>
@@ -8249,11 +8324,11 @@
       <c r="B34" s="92"/>
       <c r="C34" s="99"/>
       <c r="D34" s="201" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E34" s="202"/>
       <c r="F34" s="78" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G34" s="80" t="s">
         <v>191</v>
@@ -8271,7 +8346,7 @@
         <v>180</v>
       </c>
       <c r="L34" s="79" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="M34" s="66"/>
       <c r="N34" s="66"/>
@@ -8281,18 +8356,18 @@
       <c r="A35" s="66"/>
       <c r="B35" s="92"/>
       <c r="C35" s="95" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D35" s="96"/>
       <c r="E35" s="94"/>
       <c r="F35" s="78" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G35" s="80" t="s">
         <v>185</v>
       </c>
       <c r="H35" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I35" s="80">
         <v>1</v>
@@ -8304,7 +8379,7 @@
         <v>193</v>
       </c>
       <c r="L35" s="79" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="M35" s="66"/>
       <c r="N35" s="66"/>
@@ -8315,17 +8390,17 @@
       <c r="B36" s="92"/>
       <c r="C36" s="102"/>
       <c r="D36" s="201" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E36" s="202"/>
       <c r="F36" s="78" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G36" s="80" t="s">
         <v>194</v>
       </c>
       <c r="H36" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I36" s="80">
         <v>1</v>
@@ -8337,7 +8412,7 @@
         <v>180</v>
       </c>
       <c r="L36" s="79" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="M36" s="66"/>
       <c r="N36" s="66"/>
@@ -8347,18 +8422,18 @@
       <c r="A37" s="66"/>
       <c r="B37" s="92"/>
       <c r="C37" s="102"/>
-      <c r="D37" s="203" t="s">
-        <v>289</v>
-      </c>
-      <c r="E37" s="204"/>
+      <c r="D37" s="214" t="s">
+        <v>286</v>
+      </c>
+      <c r="E37" s="215"/>
       <c r="F37" s="78" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G37" s="80" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H37" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I37" s="80">
         <v>1</v>
@@ -8370,7 +8445,7 @@
         <v>180</v>
       </c>
       <c r="L37" s="79" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M37" s="66"/>
       <c r="N37" s="66"/>
@@ -8381,17 +8456,17 @@
       <c r="B38" s="92"/>
       <c r="C38" s="97"/>
       <c r="D38" s="201" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E38" s="202"/>
       <c r="F38" s="78" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G38" s="80" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H38" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I38" s="80">
         <v>1</v>
@@ -8403,7 +8478,7 @@
         <v>180</v>
       </c>
       <c r="L38" s="79" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="M38" s="66"/>
       <c r="N38" s="66"/>
@@ -8414,17 +8489,17 @@
       <c r="B39" s="92"/>
       <c r="C39" s="97"/>
       <c r="D39" s="71" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E39" s="73"/>
       <c r="F39" s="78" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G39" s="80" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H39" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I39" s="80">
         <v>1</v>
@@ -8436,7 +8511,7 @@
         <v>180</v>
       </c>
       <c r="L39" s="79" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="M39" s="66"/>
       <c r="N39" s="66"/>
@@ -8457,7 +8532,7 @@
         <v>191</v>
       </c>
       <c r="H40" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I40" s="80">
         <v>1</v>
@@ -8469,7 +8544,7 @@
         <v>180</v>
       </c>
       <c r="L40" s="79" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M40" s="66"/>
       <c r="N40" s="66"/>
@@ -8495,7 +8570,7 @@
     <row r="42" spans="1:15" ht="20" customHeight="1">
       <c r="A42" s="66"/>
       <c r="B42" s="33" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C42" s="93"/>
       <c r="D42" s="86"/>
@@ -8751,11 +8826,11 @@
     </row>
     <row r="57" spans="1:15" ht="20" customHeight="1">
       <c r="A57" s="66"/>
-      <c r="B57" s="215" t="s">
+      <c r="B57" s="213" t="s">
         <v>192</v>
       </c>
-      <c r="C57" s="215"/>
-      <c r="D57" s="215"/>
+      <c r="C57" s="213"/>
+      <c r="D57" s="213"/>
       <c r="E57" s="66"/>
       <c r="F57" s="66"/>
       <c r="G57" s="66"/>
@@ -8772,12 +8847,12 @@
     </row>
     <row r="58" spans="1:15" s="91" customFormat="1" ht="20" customHeight="1">
       <c r="A58" s="90"/>
-      <c r="B58" s="205" t="s">
+      <c r="B58" s="206" t="s">
         <v>173</v>
       </c>
-      <c r="C58" s="206"/>
-      <c r="D58" s="206"/>
-      <c r="E58" s="207"/>
+      <c r="C58" s="207"/>
+      <c r="D58" s="207"/>
+      <c r="E58" s="208"/>
       <c r="F58" s="76" t="s">
         <v>172</v>
       </c>
@@ -8838,18 +8913,18 @@
       <c r="A60" s="66"/>
       <c r="B60" s="92"/>
       <c r="C60" s="95" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D60" s="96"/>
       <c r="E60" s="94"/>
       <c r="F60" s="78" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G60" s="80" t="s">
         <v>185</v>
       </c>
       <c r="H60" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I60" s="80">
         <v>1</v>
@@ -8870,7 +8945,7 @@
       <c r="B61" s="92"/>
       <c r="C61" s="97"/>
       <c r="D61" s="201" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E61" s="202"/>
       <c r="F61" s="78" t="s">
@@ -8880,7 +8955,7 @@
         <v>181</v>
       </c>
       <c r="H61" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I61" s="80">
         <v>1</v>
@@ -8901,11 +8976,11 @@
       <c r="B62" s="92"/>
       <c r="C62" s="99"/>
       <c r="D62" s="201" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E62" s="202"/>
       <c r="F62" s="78" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G62" s="80" t="s">
         <v>191</v>
@@ -8923,7 +8998,7 @@
         <v>180</v>
       </c>
       <c r="L62" s="79" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="M62" s="66"/>
       <c r="N62" s="66"/>
@@ -8933,18 +9008,18 @@
       <c r="A63" s="66"/>
       <c r="B63" s="92"/>
       <c r="C63" s="95" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D63" s="96"/>
       <c r="E63" s="94"/>
       <c r="F63" s="78" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G63" s="80" t="s">
         <v>185</v>
       </c>
       <c r="H63" s="80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I63" s="80">
         <v>1</v>
@@ -8997,7 +9072,7 @@
     <row r="66" spans="1:15" ht="20" customHeight="1">
       <c r="A66" s="66"/>
       <c r="B66" s="74" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C66" s="66"/>
       <c r="D66" s="66"/>
@@ -9219,6 +9294,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B58:E58"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B30:E30"/>
@@ -9235,13 +9317,6 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B58:E58"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Update spec for "Create User Account"
</commit_message>
<xml_diff>
--- a/doc/detail_design/api/MCS_Web_API_Specification.xlsx
+++ b/doc/detail_design/api/MCS_Web_API_Specification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="-19140" windowWidth="27480" windowHeight="14520" tabRatio="957" activeTab="3"/>
+    <workbookView xWindow="5620" yWindow="-19140" windowWidth="27480" windowHeight="14520" tabRatio="957" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="23" r:id="rId1"/>
@@ -1168,7 +1168,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t>.</t>
     </r>
@@ -1189,7 +1188,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">User </t>
     </r>
@@ -1208,7 +1206,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t>ccount</t>
     </r>
@@ -1222,14 +1219,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1237,7 +1234,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1245,7 +1242,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1258,45 +1255,45 @@
     <font>
       <sz val="18"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF963634"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1311,7 +1308,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2457,44 +2454,72 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2526,16 +2551,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2563,21 +2578,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -2590,22 +2590,43 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2620,6 +2641,9 @@
     <xf numFmtId="0" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2655,21 +2679,19 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2685,42 +2707,17 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="411">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3928,7 +3925,16 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>      "message": "Success"</a:t>
+            <a:t>      "description": "User account was created successfully.",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>      "message": "Account created success!"</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4795,299 +4801,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="43" customFormat="1">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="163" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="187" t="s">
+      <c r="B1" s="164"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="192" t="s">
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="193"/>
-      <c r="M1" s="194"/>
-      <c r="N1" s="174" t="s">
+      <c r="L1" s="169"/>
+      <c r="M1" s="170"/>
+      <c r="N1" s="171" t="s">
         <v>191</v>
       </c>
-      <c r="O1" s="175"/>
-      <c r="P1" s="175"/>
-      <c r="Q1" s="175"/>
-      <c r="R1" s="175"/>
-      <c r="S1" s="175"/>
-      <c r="T1" s="175"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="195" t="s">
+      <c r="O1" s="172"/>
+      <c r="P1" s="172"/>
+      <c r="Q1" s="172"/>
+      <c r="R1" s="172"/>
+      <c r="S1" s="172"/>
+      <c r="T1" s="172"/>
+      <c r="U1" s="173"/>
+      <c r="V1" s="174" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="196"/>
-      <c r="X1" s="196"/>
-      <c r="Y1" s="196"/>
-      <c r="Z1" s="196"/>
-      <c r="AA1" s="196"/>
-      <c r="AB1" s="196"/>
-      <c r="AC1" s="196"/>
-      <c r="AD1" s="197"/>
+      <c r="W1" s="175"/>
+      <c r="X1" s="175"/>
+      <c r="Y1" s="175"/>
+      <c r="Z1" s="175"/>
+      <c r="AA1" s="175"/>
+      <c r="AB1" s="175"/>
+      <c r="AC1" s="175"/>
+      <c r="AD1" s="176"/>
     </row>
     <row r="2" spans="1:30" s="43" customFormat="1">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="163" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="187" t="s">
+      <c r="B2" s="164"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="166" t="s">
         <v>194</v>
       </c>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
-      <c r="J2" s="188"/>
-      <c r="K2" s="169" t="s">
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="180" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="170"/>
-      <c r="M2" s="171"/>
-      <c r="N2" s="189" t="s">
+      <c r="L2" s="181"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="192" t="s">
         <v>196</v>
       </c>
-      <c r="O2" s="190"/>
-      <c r="P2" s="190"/>
-      <c r="Q2" s="190"/>
-      <c r="R2" s="190"/>
-      <c r="S2" s="190"/>
-      <c r="T2" s="190"/>
-      <c r="U2" s="191"/>
-      <c r="V2" s="166" t="s">
+      <c r="O2" s="193"/>
+      <c r="P2" s="193"/>
+      <c r="Q2" s="193"/>
+      <c r="R2" s="193"/>
+      <c r="S2" s="193"/>
+      <c r="T2" s="193"/>
+      <c r="U2" s="194"/>
+      <c r="V2" s="177" t="s">
         <v>198</v>
       </c>
-      <c r="W2" s="167"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="166" t="s">
+      <c r="W2" s="178"/>
+      <c r="X2" s="179"/>
+      <c r="Y2" s="177" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="167"/>
-      <c r="AA2" s="168"/>
-      <c r="AB2" s="166" t="s">
+      <c r="Z2" s="178"/>
+      <c r="AA2" s="179"/>
+      <c r="AB2" s="177" t="s">
         <v>43</v>
       </c>
-      <c r="AC2" s="167"/>
-      <c r="AD2" s="168"/>
+      <c r="AC2" s="178"/>
+      <c r="AD2" s="179"/>
     </row>
     <row r="3" spans="1:30" s="43" customFormat="1">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="170"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="172" t="s">
+      <c r="B3" s="181"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="183" t="s">
         <v>195</v>
       </c>
-      <c r="E3" s="173"/>
-      <c r="F3" s="173"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="173"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="173"/>
-      <c r="K3" s="169" t="s">
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="180" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="170"/>
-      <c r="M3" s="171"/>
-      <c r="N3" s="174" t="s">
+      <c r="L3" s="181"/>
+      <c r="M3" s="182"/>
+      <c r="N3" s="171" t="s">
         <v>197</v>
       </c>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="176"/>
-      <c r="V3" s="177" t="s">
+      <c r="O3" s="172"/>
+      <c r="P3" s="172"/>
+      <c r="Q3" s="172"/>
+      <c r="R3" s="172"/>
+      <c r="S3" s="172"/>
+      <c r="T3" s="172"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="185" t="s">
         <v>199</v>
       </c>
-      <c r="W3" s="178"/>
-      <c r="X3" s="179"/>
-      <c r="Y3" s="180"/>
-      <c r="Z3" s="181"/>
-      <c r="AA3" s="182"/>
-      <c r="AB3" s="183"/>
-      <c r="AC3" s="181"/>
-      <c r="AD3" s="182"/>
+      <c r="W3" s="186"/>
+      <c r="X3" s="187"/>
+      <c r="Y3" s="188"/>
+      <c r="Z3" s="189"/>
+      <c r="AA3" s="190"/>
+      <c r="AB3" s="191"/>
+      <c r="AC3" s="189"/>
+      <c r="AD3" s="190"/>
     </row>
     <row r="7" spans="1:30" ht="16" thickBot="1"/>
     <row r="8" spans="1:30" ht="16" thickBot="1">
-      <c r="B8" s="164" t="s">
+      <c r="B8" s="207" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164" t="s">
+      <c r="C8" s="207"/>
+      <c r="D8" s="207"/>
+      <c r="E8" s="207"/>
+      <c r="F8" s="207" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="164"/>
-      <c r="H8" s="164" t="s">
+      <c r="G8" s="207"/>
+      <c r="H8" s="207" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="164"/>
-      <c r="J8" s="164"/>
-      <c r="K8" s="164" t="s">
+      <c r="I8" s="207"/>
+      <c r="J8" s="207"/>
+      <c r="K8" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="164"/>
-      <c r="M8" s="164"/>
-      <c r="N8" s="164"/>
-      <c r="O8" s="164"/>
-      <c r="P8" s="164"/>
-      <c r="Q8" s="164"/>
-      <c r="R8" s="164"/>
-      <c r="S8" s="164"/>
-      <c r="T8" s="164"/>
-      <c r="U8" s="164"/>
-      <c r="V8" s="164"/>
-      <c r="W8" s="164"/>
-      <c r="X8" s="164" t="s">
+      <c r="L8" s="207"/>
+      <c r="M8" s="207"/>
+      <c r="N8" s="207"/>
+      <c r="O8" s="207"/>
+      <c r="P8" s="207"/>
+      <c r="Q8" s="207"/>
+      <c r="R8" s="207"/>
+      <c r="S8" s="207"/>
+      <c r="T8" s="207"/>
+      <c r="U8" s="207"/>
+      <c r="V8" s="207"/>
+      <c r="W8" s="207"/>
+      <c r="X8" s="207" t="s">
         <v>47</v>
       </c>
-      <c r="Y8" s="164"/>
-      <c r="Z8" s="164"/>
-      <c r="AA8" s="164"/>
-      <c r="AB8" s="164"/>
-      <c r="AC8" s="164"/>
+      <c r="Y8" s="207"/>
+      <c r="Z8" s="207"/>
+      <c r="AA8" s="207"/>
+      <c r="AB8" s="207"/>
+      <c r="AC8" s="207"/>
     </row>
     <row r="9" spans="1:30">
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="195" t="s">
         <v>193</v>
       </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="156" t="s">
+      <c r="C9" s="196"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="198" t="s">
         <v>190</v>
       </c>
-      <c r="G9" s="157"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="155"/>
-      <c r="K9" s="158"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="159"/>
-      <c r="S9" s="159"/>
-      <c r="T9" s="159"/>
-      <c r="U9" s="159"/>
-      <c r="V9" s="159"/>
-      <c r="W9" s="160"/>
-      <c r="X9" s="161"/>
-      <c r="Y9" s="162"/>
-      <c r="Z9" s="162"/>
-      <c r="AA9" s="162"/>
-      <c r="AB9" s="162"/>
-      <c r="AC9" s="163"/>
+      <c r="G9" s="199"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="196"/>
+      <c r="J9" s="197"/>
+      <c r="K9" s="201"/>
+      <c r="L9" s="202"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="202"/>
+      <c r="O9" s="202"/>
+      <c r="P9" s="202"/>
+      <c r="Q9" s="202"/>
+      <c r="R9" s="202"/>
+      <c r="S9" s="202"/>
+      <c r="T9" s="202"/>
+      <c r="U9" s="202"/>
+      <c r="V9" s="202"/>
+      <c r="W9" s="203"/>
+      <c r="X9" s="204"/>
+      <c r="Y9" s="205"/>
+      <c r="Z9" s="205"/>
+      <c r="AA9" s="205"/>
+      <c r="AB9" s="205"/>
+      <c r="AC9" s="206"/>
     </row>
     <row r="10" spans="1:30">
-      <c r="B10" s="153"/>
-      <c r="C10" s="154"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="155"/>
-      <c r="F10" s="156"/>
-      <c r="G10" s="157"/>
-      <c r="H10" s="153"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="155"/>
-      <c r="K10" s="158"/>
-      <c r="L10" s="159"/>
-      <c r="M10" s="159"/>
-      <c r="N10" s="159"/>
-      <c r="O10" s="159"/>
-      <c r="P10" s="159"/>
-      <c r="Q10" s="159"/>
-      <c r="R10" s="159"/>
-      <c r="S10" s="159"/>
-      <c r="T10" s="159"/>
-      <c r="U10" s="159"/>
-      <c r="V10" s="159"/>
-      <c r="W10" s="160"/>
-      <c r="X10" s="161"/>
-      <c r="Y10" s="162"/>
-      <c r="Z10" s="162"/>
-      <c r="AA10" s="162"/>
-      <c r="AB10" s="162"/>
-      <c r="AC10" s="163"/>
+      <c r="B10" s="200"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="198"/>
+      <c r="G10" s="199"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="196"/>
+      <c r="J10" s="197"/>
+      <c r="K10" s="201"/>
+      <c r="L10" s="202"/>
+      <c r="M10" s="202"/>
+      <c r="N10" s="202"/>
+      <c r="O10" s="202"/>
+      <c r="P10" s="202"/>
+      <c r="Q10" s="202"/>
+      <c r="R10" s="202"/>
+      <c r="S10" s="202"/>
+      <c r="T10" s="202"/>
+      <c r="U10" s="202"/>
+      <c r="V10" s="202"/>
+      <c r="W10" s="203"/>
+      <c r="X10" s="204"/>
+      <c r="Y10" s="205"/>
+      <c r="Z10" s="205"/>
+      <c r="AA10" s="205"/>
+      <c r="AB10" s="205"/>
+      <c r="AC10" s="206"/>
     </row>
     <row r="11" spans="1:30">
-      <c r="B11" s="153"/>
-      <c r="C11" s="154"/>
-      <c r="D11" s="154"/>
-      <c r="E11" s="155"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="154"/>
-      <c r="J11" s="155"/>
-      <c r="K11" s="158"/>
-      <c r="L11" s="159"/>
-      <c r="M11" s="159"/>
-      <c r="N11" s="159"/>
-      <c r="O11" s="159"/>
-      <c r="P11" s="159"/>
-      <c r="Q11" s="159"/>
-      <c r="R11" s="159"/>
-      <c r="S11" s="159"/>
-      <c r="T11" s="159"/>
-      <c r="U11" s="159"/>
-      <c r="V11" s="159"/>
-      <c r="W11" s="160"/>
-      <c r="X11" s="161"/>
-      <c r="Y11" s="162"/>
-      <c r="Z11" s="162"/>
-      <c r="AA11" s="162"/>
-      <c r="AB11" s="162"/>
-      <c r="AC11" s="163"/>
+      <c r="B11" s="200"/>
+      <c r="C11" s="196"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="198"/>
+      <c r="G11" s="199"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="196"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="201"/>
+      <c r="L11" s="202"/>
+      <c r="M11" s="202"/>
+      <c r="N11" s="202"/>
+      <c r="O11" s="202"/>
+      <c r="P11" s="202"/>
+      <c r="Q11" s="202"/>
+      <c r="R11" s="202"/>
+      <c r="S11" s="202"/>
+      <c r="T11" s="202"/>
+      <c r="U11" s="202"/>
+      <c r="V11" s="202"/>
+      <c r="W11" s="203"/>
+      <c r="X11" s="204"/>
+      <c r="Y11" s="205"/>
+      <c r="Z11" s="205"/>
+      <c r="AA11" s="205"/>
+      <c r="AB11" s="205"/>
+      <c r="AC11" s="206"/>
     </row>
     <row r="12" spans="1:30">
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="155"/>
-      <c r="F12" s="156"/>
-      <c r="G12" s="157"/>
-      <c r="H12" s="153"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="155"/>
-      <c r="K12" s="158"/>
-      <c r="L12" s="159"/>
-      <c r="M12" s="159"/>
-      <c r="N12" s="159"/>
-      <c r="O12" s="159"/>
-      <c r="P12" s="159"/>
-      <c r="Q12" s="159"/>
-      <c r="R12" s="159"/>
-      <c r="S12" s="159"/>
-      <c r="T12" s="159"/>
-      <c r="U12" s="159"/>
-      <c r="V12" s="159"/>
-      <c r="W12" s="160"/>
-      <c r="X12" s="161"/>
-      <c r="Y12" s="162"/>
-      <c r="Z12" s="162"/>
-      <c r="AA12" s="162"/>
-      <c r="AB12" s="162"/>
-      <c r="AC12" s="163"/>
+      <c r="B12" s="200"/>
+      <c r="C12" s="196"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="197"/>
+      <c r="F12" s="198"/>
+      <c r="G12" s="199"/>
+      <c r="H12" s="200"/>
+      <c r="I12" s="196"/>
+      <c r="J12" s="197"/>
+      <c r="K12" s="201"/>
+      <c r="L12" s="202"/>
+      <c r="M12" s="202"/>
+      <c r="N12" s="202"/>
+      <c r="O12" s="202"/>
+      <c r="P12" s="202"/>
+      <c r="Q12" s="202"/>
+      <c r="R12" s="202"/>
+      <c r="S12" s="202"/>
+      <c r="T12" s="202"/>
+      <c r="U12" s="202"/>
+      <c r="V12" s="202"/>
+      <c r="W12" s="203"/>
+      <c r="X12" s="204"/>
+      <c r="Y12" s="205"/>
+      <c r="Z12" s="205"/>
+      <c r="AA12" s="205"/>
+      <c r="AB12" s="205"/>
+      <c r="AC12" s="206"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1"/>
     <row r="14" spans="1:30" ht="18" customHeight="1"/>
@@ -5117,11 +5123,31 @@
     <row r="38" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:W12"/>
+    <mergeCell ref="X12:AC12"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:W10"/>
+    <mergeCell ref="X10:AC10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:W11"/>
+    <mergeCell ref="X11:AC11"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:W8"/>
+    <mergeCell ref="X8:AC8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:W9"/>
+    <mergeCell ref="X9:AC9"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="A3:C3"/>
@@ -5136,31 +5162,11 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:U2"/>
     <mergeCell ref="V2:X2"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:W9"/>
-    <mergeCell ref="X9:AC9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:W8"/>
-    <mergeCell ref="X8:AC8"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:W11"/>
-    <mergeCell ref="X11:AC11"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:W10"/>
-    <mergeCell ref="X10:AC10"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:W12"/>
-    <mergeCell ref="X12:AC12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AD1"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5181,7 +5187,7 @@
       <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
@@ -5199,10 +5205,10 @@
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
     </row>
-    <row r="3" spans="2:6" ht="16">
+    <row r="3" spans="2:6">
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="2:6" ht="18">
+    <row r="4" spans="2:6" ht="20">
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
@@ -5210,7 +5216,7 @@
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
     </row>
-    <row r="5" spans="2:6" ht="18">
+    <row r="5" spans="2:6" ht="20">
       <c r="C5" s="7" t="s">
         <v>50</v>
       </c>
@@ -5218,7 +5224,7 @@
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
     </row>
-    <row r="6" spans="2:6" ht="18">
+    <row r="6" spans="2:6" ht="20">
       <c r="C6" s="8" t="s">
         <v>35</v>
       </c>
@@ -5232,7 +5238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="18">
+    <row r="7" spans="2:6" ht="20">
       <c r="C7" s="7">
         <v>1</v>
       </c>
@@ -5246,7 +5252,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="18">
+    <row r="8" spans="2:6" ht="20">
       <c r="C8" s="7">
         <v>2</v>
       </c>
@@ -5260,19 +5266,19 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="18">
+    <row r="9" spans="2:6" ht="20">
       <c r="C9" s="7"/>
       <c r="D9" s="11"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
     </row>
-    <row r="10" spans="2:6" ht="18">
+    <row r="10" spans="2:6" ht="20">
       <c r="C10" s="7"/>
       <c r="D10" s="12"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
     </row>
-    <row r="11" spans="2:6" ht="18">
+    <row r="11" spans="2:6" ht="20">
       <c r="C11" s="13" t="s">
         <v>56</v>
       </c>
@@ -5280,7 +5286,7 @@
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
     </row>
-    <row r="12" spans="2:6" ht="18">
+    <row r="12" spans="2:6" ht="20">
       <c r="C12" s="14" t="s">
         <v>57</v>
       </c>
@@ -5288,7 +5294,7 @@
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
     </row>
-    <row r="13" spans="2:6" ht="18">
+    <row r="13" spans="2:6" ht="20">
       <c r="C13" s="8" t="s">
         <v>35</v>
       </c>
@@ -5302,7 +5308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="18">
+    <row r="14" spans="2:6" ht="20">
       <c r="C14" s="7">
         <v>1</v>
       </c>
@@ -5316,7 +5322,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="18">
+    <row r="15" spans="2:6" ht="20">
       <c r="C15" s="7">
         <v>2</v>
       </c>
@@ -5330,7 +5336,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="18">
+    <row r="16" spans="2:6" ht="20">
       <c r="C16" s="7">
         <v>3</v>
       </c>
@@ -5344,13 +5350,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="18">
+    <row r="17" spans="3:6" ht="20">
       <c r="C17" s="7"/>
       <c r="D17" s="6"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
     </row>
-    <row r="18" spans="3:6" ht="18">
+    <row r="18" spans="3:6" ht="20">
       <c r="C18" s="15" t="s">
         <v>61</v>
       </c>
@@ -5358,7 +5364,7 @@
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
     </row>
-    <row r="19" spans="3:6" ht="18">
+    <row r="19" spans="3:6" ht="20">
       <c r="C19" s="17" t="s">
         <v>62</v>
       </c>
@@ -5366,7 +5372,7 @@
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
     </row>
-    <row r="20" spans="3:6" ht="18">
+    <row r="20" spans="3:6" ht="20">
       <c r="C20" s="18" t="s">
         <v>35</v>
       </c>
@@ -5380,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:6" ht="18">
+    <row r="21" spans="3:6" ht="20">
       <c r="C21" s="20">
         <v>1</v>
       </c>
@@ -5394,7 +5400,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="3:6" ht="18">
+    <row r="22" spans="3:6" ht="20">
       <c r="C22" s="20">
         <v>2</v>
       </c>
@@ -5408,7 +5414,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="3:6" ht="18">
+    <row r="23" spans="3:6" ht="20">
       <c r="C23" s="20">
         <v>3</v>
       </c>
@@ -5422,7 +5428,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="18">
+    <row r="24" spans="3:6" ht="20">
       <c r="C24" s="20">
         <v>4</v>
       </c>
@@ -5436,7 +5442,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="3:6" ht="18">
+    <row r="25" spans="3:6" ht="20">
       <c r="C25" s="20">
         <v>5</v>
       </c>
@@ -5450,7 +5456,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="3:6" ht="18">
+    <row r="28" spans="3:6" ht="20">
       <c r="C28" s="15" t="s">
         <v>83</v>
       </c>
@@ -5458,7 +5464,7 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
     </row>
-    <row r="29" spans="3:6" ht="18">
+    <row r="29" spans="3:6" ht="20">
       <c r="C29" s="17" t="s">
         <v>85</v>
       </c>
@@ -5466,7 +5472,7 @@
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
     </row>
-    <row r="30" spans="3:6" ht="18">
+    <row r="30" spans="3:6" ht="20">
       <c r="C30" s="18" t="s">
         <v>35</v>
       </c>
@@ -5480,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:6" ht="18">
+    <row r="31" spans="3:6" ht="20">
       <c r="C31" s="20">
         <v>1</v>
       </c>
@@ -5494,7 +5500,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="3:6" ht="18">
+    <row r="32" spans="3:6" ht="20">
       <c r="C32" s="20">
         <v>2</v>
       </c>
@@ -5508,19 +5514,19 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="3:6" ht="18">
+    <row r="33" spans="3:6" ht="20">
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
       <c r="E33" s="26"/>
       <c r="F33" s="32"/>
     </row>
-    <row r="34" spans="3:6" ht="18">
+    <row r="34" spans="3:6" ht="20">
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
       <c r="E34" s="26"/>
       <c r="F34" s="32"/>
     </row>
-    <row r="35" spans="3:6" ht="18">
+    <row r="35" spans="3:6" ht="20">
       <c r="C35" s="15" t="s">
         <v>78</v>
       </c>
@@ -5528,7 +5534,7 @@
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
     </row>
-    <row r="36" spans="3:6" ht="18">
+    <row r="36" spans="3:6" ht="20">
       <c r="C36" s="17" t="s">
         <v>79</v>
       </c>
@@ -5536,7 +5542,7 @@
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
     </row>
-    <row r="37" spans="3:6" ht="18">
+    <row r="37" spans="3:6" ht="20">
       <c r="C37" s="18" t="s">
         <v>35</v>
       </c>
@@ -5550,7 +5556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:6" ht="18">
+    <row r="38" spans="3:6" ht="20">
       <c r="C38" s="20">
         <v>1</v>
       </c>
@@ -5564,7 +5570,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="3:6" ht="18">
+    <row r="39" spans="3:6" ht="20">
       <c r="C39" s="20">
         <v>2</v>
       </c>
@@ -5578,7 +5584,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="3:6" ht="18">
+    <row r="40" spans="3:6" ht="20">
       <c r="C40" s="20">
         <v>3</v>
       </c>
@@ -5592,7 +5598,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="3:6" ht="18">
+    <row r="43" spans="3:6" ht="20">
       <c r="C43" s="15" t="s">
         <v>72</v>
       </c>
@@ -5600,7 +5606,7 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
     </row>
-    <row r="44" spans="3:6" ht="18">
+    <row r="44" spans="3:6" ht="20">
       <c r="C44" s="17" t="s">
         <v>71</v>
       </c>
@@ -5608,7 +5614,7 @@
       <c r="E44" s="28"/>
       <c r="F44" s="28"/>
     </row>
-    <row r="45" spans="3:6" ht="18">
+    <row r="45" spans="3:6" ht="20">
       <c r="C45" s="18" t="s">
         <v>35</v>
       </c>
@@ -5622,7 +5628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:6" ht="18">
+    <row r="46" spans="3:6" ht="20">
       <c r="C46" s="20">
         <v>1</v>
       </c>
@@ -5636,7 +5642,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="3:6" ht="18">
+    <row r="47" spans="3:6" ht="20">
       <c r="C47" s="20">
         <v>2</v>
       </c>
@@ -5650,7 +5656,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="3:6" ht="18">
+    <row r="50" spans="3:6" ht="20">
       <c r="C50" s="15" t="s">
         <v>73</v>
       </c>
@@ -5658,7 +5664,7 @@
       <c r="E50" s="28"/>
       <c r="F50" s="28"/>
     </row>
-    <row r="51" spans="3:6" ht="18">
+    <row r="51" spans="3:6" ht="20">
       <c r="C51" s="17" t="s">
         <v>74</v>
       </c>
@@ -5666,7 +5672,7 @@
       <c r="E51" s="28"/>
       <c r="F51" s="28"/>
     </row>
-    <row r="52" spans="3:6" ht="18">
+    <row r="52" spans="3:6" ht="20">
       <c r="C52" s="18" t="s">
         <v>35</v>
       </c>
@@ -5680,7 +5686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:6" ht="18">
+    <row r="53" spans="3:6" ht="20">
       <c r="C53" s="20">
         <v>1</v>
       </c>
@@ -5694,7 +5700,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="3:6" ht="18">
+    <row r="56" spans="3:6" ht="20">
       <c r="C56" s="15" t="s">
         <v>157</v>
       </c>
@@ -5702,7 +5708,7 @@
       <c r="E56" s="28"/>
       <c r="F56" s="28"/>
     </row>
-    <row r="57" spans="3:6" ht="18">
+    <row r="57" spans="3:6" ht="20">
       <c r="C57" s="17" t="s">
         <v>158</v>
       </c>
@@ -5710,7 +5716,7 @@
       <c r="E57" s="28"/>
       <c r="F57" s="28"/>
     </row>
-    <row r="58" spans="3:6" ht="18">
+    <row r="58" spans="3:6" ht="20">
       <c r="C58" s="18" t="s">
         <v>35</v>
       </c>
@@ -5724,7 +5730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:6" ht="18">
+    <row r="59" spans="3:6" ht="20">
       <c r="C59" s="20">
         <v>1</v>
       </c>
@@ -6210,7 +6216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -6265,10 +6271,10 @@
       <c r="C4" s="104" t="s">
         <v>350</v>
       </c>
-      <c r="D4" s="199" t="s">
+      <c r="D4" s="209" t="s">
         <v>354</v>
       </c>
-      <c r="E4" s="199"/>
+      <c r="E4" s="209"/>
       <c r="F4" s="150" t="s">
         <v>351</v>
       </c>
@@ -6280,17 +6286,17 @@
       <c r="L4" s="122"/>
     </row>
     <row r="5" spans="2:12" ht="20" customHeight="1">
-      <c r="B5" s="227">
+      <c r="B5" s="153">
         <v>1</v>
       </c>
-      <c r="C5" s="228" t="s">
+      <c r="C5" s="154" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="229" t="s">
+      <c r="D5" s="212" t="s">
         <v>356</v>
       </c>
-      <c r="E5" s="229"/>
-      <c r="F5" s="230" t="s">
+      <c r="E5" s="212"/>
+      <c r="F5" s="155" t="s">
         <v>355</v>
       </c>
       <c r="G5" s="125"/>
@@ -6344,10 +6350,10 @@
       <c r="C9" s="150" t="s">
         <v>350</v>
       </c>
-      <c r="D9" s="199" t="s">
+      <c r="D9" s="209" t="s">
         <v>354</v>
       </c>
-      <c r="E9" s="199"/>
+      <c r="E9" s="209"/>
       <c r="F9" s="150" t="s">
         <v>351</v>
       </c>
@@ -6359,10 +6365,10 @@
       <c r="C10" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="198" t="s">
+      <c r="D10" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="198"/>
+      <c r="E10" s="208"/>
       <c r="F10" s="148"/>
       <c r="G10" s="125" t="s">
         <v>326</v>
@@ -6376,10 +6382,10 @@
       <c r="C11" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="198" t="s">
+      <c r="D11" s="208" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="198"/>
+      <c r="E11" s="208"/>
       <c r="F11" s="148"/>
       <c r="G11" s="125"/>
       <c r="H11" s="125"/>
@@ -6391,10 +6397,10 @@
       <c r="C12" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="198" t="s">
+      <c r="D12" s="208" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="198"/>
+      <c r="E12" s="208"/>
       <c r="F12" s="148"/>
       <c r="G12" s="125"/>
       <c r="H12" s="125"/>
@@ -6406,10 +6412,10 @@
       <c r="C13" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="198" t="s">
+      <c r="D13" s="208" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="198"/>
+      <c r="E13" s="208"/>
       <c r="F13" s="148"/>
       <c r="G13" s="125"/>
       <c r="H13" s="125"/>
@@ -6421,10 +6427,10 @@
       <c r="C14" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="198" t="s">
+      <c r="D14" s="208" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="198"/>
+      <c r="E14" s="208"/>
       <c r="F14" s="148"/>
       <c r="G14" s="125"/>
       <c r="H14" s="125"/>
@@ -6436,10 +6442,10 @@
       <c r="C15" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="198" t="s">
+      <c r="D15" s="208" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="198"/>
+      <c r="E15" s="208"/>
       <c r="F15" s="148"/>
       <c r="G15" s="125"/>
       <c r="H15" s="125"/>
@@ -6459,10 +6465,10 @@
       <c r="C18" s="150" t="s">
         <v>350</v>
       </c>
-      <c r="D18" s="199" t="s">
+      <c r="D18" s="209" t="s">
         <v>354</v>
       </c>
-      <c r="E18" s="199"/>
+      <c r="E18" s="209"/>
       <c r="F18" s="150" t="s">
         <v>351</v>
       </c>
@@ -6474,10 +6480,10 @@
       <c r="C19" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="198" t="s">
+      <c r="D19" s="208" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="198"/>
+      <c r="E19" s="208"/>
       <c r="F19" s="152"/>
       <c r="G19" s="125"/>
       <c r="H19" s="125"/>
@@ -6489,10 +6495,10 @@
       <c r="C20" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="198" t="s">
+      <c r="D20" s="208" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="198"/>
+      <c r="E20" s="208"/>
       <c r="F20" s="152"/>
       <c r="G20" s="125"/>
       <c r="H20" s="125"/>
@@ -6504,10 +6510,10 @@
       <c r="C21" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="198" t="s">
+      <c r="D21" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="198"/>
+      <c r="E21" s="208"/>
       <c r="F21" s="152"/>
       <c r="G21" s="125"/>
       <c r="H21" s="125"/>
@@ -6519,10 +6525,10 @@
       <c r="C22" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="198" t="s">
+      <c r="D22" s="208" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="198"/>
+      <c r="E22" s="208"/>
       <c r="F22" s="152"/>
       <c r="G22" s="125"/>
       <c r="H22" s="125"/>
@@ -6534,10 +6540,10 @@
       <c r="C23" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="198" t="s">
+      <c r="D23" s="208" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="198"/>
+      <c r="E23" s="208"/>
       <c r="F23" s="152"/>
       <c r="G23" s="125"/>
       <c r="H23" s="125"/>
@@ -6549,10 +6555,10 @@
       <c r="C24" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="198" t="s">
+      <c r="D24" s="208" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="198"/>
+      <c r="E24" s="208"/>
       <c r="F24" s="152"/>
       <c r="G24" s="125"/>
       <c r="H24" s="125"/>
@@ -6572,26 +6578,26 @@
       <c r="C27" s="150" t="s">
         <v>350</v>
       </c>
-      <c r="D27" s="199" t="s">
+      <c r="D27" s="209" t="s">
         <v>354</v>
       </c>
-      <c r="E27" s="199"/>
+      <c r="E27" s="209"/>
       <c r="F27" s="150" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="20" customHeight="1">
-      <c r="B28" s="227">
+      <c r="B28" s="153">
         <v>1</v>
       </c>
-      <c r="C28" s="228" t="s">
+      <c r="C28" s="154" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="229" t="s">
+      <c r="D28" s="212" t="s">
         <v>353</v>
       </c>
-      <c r="E28" s="229"/>
-      <c r="F28" s="231"/>
+      <c r="E28" s="212"/>
+      <c r="F28" s="156"/>
       <c r="G28" s="125"/>
       <c r="H28" s="125"/>
     </row>
@@ -6602,10 +6608,10 @@
       <c r="C29" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="198" t="s">
+      <c r="D29" s="208" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="198"/>
+      <c r="E29" s="208"/>
       <c r="F29" s="152"/>
       <c r="G29" s="125"/>
       <c r="H29" s="125"/>
@@ -6617,10 +6623,10 @@
       <c r="C30" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="198" t="s">
+      <c r="D30" s="208" t="s">
         <v>97</v>
       </c>
-      <c r="E30" s="198"/>
+      <c r="E30" s="208"/>
       <c r="F30" s="152"/>
       <c r="G30" s="125"/>
       <c r="H30" s="125"/>
@@ -6632,10 +6638,10 @@
       <c r="C31" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="198" t="s">
+      <c r="D31" s="208" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="198"/>
+      <c r="E31" s="208"/>
       <c r="F31" s="152"/>
       <c r="G31" s="125"/>
       <c r="H31" s="125"/>
@@ -6647,10 +6653,10 @@
       <c r="C32" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="198" t="s">
+      <c r="D32" s="208" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="198"/>
+      <c r="E32" s="208"/>
       <c r="F32" s="152"/>
       <c r="G32" s="125"/>
       <c r="H32" s="125"/>
@@ -6662,10 +6668,10 @@
       <c r="C33" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="198" t="s">
+      <c r="D33" s="208" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="198"/>
+      <c r="E33" s="208"/>
       <c r="F33" s="152"/>
       <c r="G33" s="125"/>
       <c r="H33" s="125"/>
@@ -6677,10 +6683,10 @@
       <c r="C34" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="198" t="s">
+      <c r="D34" s="208" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="198"/>
+      <c r="E34" s="208"/>
       <c r="F34" s="152"/>
       <c r="G34" s="125"/>
       <c r="H34" s="125"/>
@@ -6692,10 +6698,10 @@
       <c r="C35" s="127" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="198" t="s">
+      <c r="D35" s="208" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="198"/>
+      <c r="E35" s="208"/>
       <c r="F35" s="152"/>
       <c r="G35" s="125"/>
       <c r="H35" s="125"/>
@@ -6707,10 +6713,10 @@
       <c r="C36" s="127" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="198" t="s">
+      <c r="D36" s="208" t="s">
         <v>107</v>
       </c>
-      <c r="E36" s="198"/>
+      <c r="E36" s="208"/>
       <c r="F36" s="152"/>
       <c r="G36" s="125"/>
       <c r="H36" s="125"/>
@@ -6728,10 +6734,10 @@
       <c r="C40" s="150" t="s">
         <v>350</v>
       </c>
-      <c r="D40" s="199" t="s">
+      <c r="D40" s="209" t="s">
         <v>354</v>
       </c>
-      <c r="E40" s="199"/>
+      <c r="E40" s="209"/>
       <c r="F40" s="150" t="s">
         <v>351</v>
       </c>
@@ -6743,10 +6749,10 @@
       <c r="C41" s="127" t="s">
         <v>146</v>
       </c>
-      <c r="D41" s="200" t="s">
+      <c r="D41" s="210" t="s">
         <v>151</v>
       </c>
-      <c r="E41" s="201"/>
+      <c r="E41" s="211"/>
       <c r="F41" s="149"/>
     </row>
     <row r="42" spans="2:8" ht="15" customHeight="1">
@@ -6756,10 +6762,10 @@
       <c r="C42" s="127" t="s">
         <v>147</v>
       </c>
-      <c r="D42" s="200" t="s">
+      <c r="D42" s="210" t="s">
         <v>156</v>
       </c>
-      <c r="E42" s="201"/>
+      <c r="E42" s="211"/>
       <c r="F42" s="149"/>
     </row>
     <row r="43" spans="2:8">
@@ -6769,8 +6775,8 @@
       <c r="C43" s="127" t="s">
         <v>148</v>
       </c>
-      <c r="D43" s="200"/>
-      <c r="E43" s="201"/>
+      <c r="D43" s="210"/>
+      <c r="E43" s="211"/>
       <c r="F43" s="149"/>
     </row>
     <row r="44" spans="2:8">
@@ -6780,8 +6786,8 @@
       <c r="C44" s="127" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="200"/>
-      <c r="E44" s="201"/>
+      <c r="D44" s="210"/>
+      <c r="E44" s="211"/>
       <c r="F44" s="149"/>
     </row>
     <row r="45" spans="2:8">
@@ -6791,8 +6797,8 @@
       <c r="C45" s="127" t="s">
         <v>150</v>
       </c>
-      <c r="D45" s="200"/>
-      <c r="E45" s="201"/>
+      <c r="D45" s="210"/>
+      <c r="E45" s="211"/>
       <c r="F45" s="149"/>
     </row>
     <row r="48" spans="2:8">
@@ -6808,10 +6814,10 @@
       <c r="C49" s="150" t="s">
         <v>350</v>
       </c>
-      <c r="D49" s="199" t="s">
+      <c r="D49" s="209" t="s">
         <v>354</v>
       </c>
-      <c r="E49" s="199"/>
+      <c r="E49" s="209"/>
       <c r="F49" s="150" t="s">
         <v>351</v>
       </c>
@@ -6823,10 +6829,10 @@
       <c r="C50" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="198" t="s">
+      <c r="D50" s="208" t="s">
         <v>115</v>
       </c>
-      <c r="E50" s="198"/>
+      <c r="E50" s="208"/>
       <c r="F50" s="152"/>
     </row>
     <row r="51" spans="2:6" ht="20" customHeight="1">
@@ -6836,10 +6842,10 @@
       <c r="C51" s="127" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="198" t="s">
+      <c r="D51" s="208" t="s">
         <v>123</v>
       </c>
-      <c r="E51" s="198"/>
+      <c r="E51" s="208"/>
       <c r="F51" s="152"/>
     </row>
     <row r="52" spans="2:6" ht="20" customHeight="1">
@@ -6849,10 +6855,10 @@
       <c r="C52" s="127" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="198" t="s">
+      <c r="D52" s="208" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="198"/>
+      <c r="E52" s="208"/>
       <c r="F52" s="152"/>
     </row>
     <row r="53" spans="2:6" ht="20" customHeight="1">
@@ -6862,10 +6868,10 @@
       <c r="C53" s="127" t="s">
         <v>119</v>
       </c>
-      <c r="D53" s="198" t="s">
+      <c r="D53" s="208" t="s">
         <v>125</v>
       </c>
-      <c r="E53" s="198"/>
+      <c r="E53" s="208"/>
       <c r="F53" s="152"/>
     </row>
     <row r="54" spans="2:6" ht="20" customHeight="1">
@@ -6875,10 +6881,10 @@
       <c r="C54" s="127" t="s">
         <v>120</v>
       </c>
-      <c r="D54" s="198" t="s">
+      <c r="D54" s="208" t="s">
         <v>126</v>
       </c>
-      <c r="E54" s="198"/>
+      <c r="E54" s="208"/>
       <c r="F54" s="152"/>
     </row>
     <row r="55" spans="2:6" ht="20" customHeight="1">
@@ -6888,10 +6894,10 @@
       <c r="C55" s="127" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="198" t="s">
+      <c r="D55" s="208" t="s">
         <v>127</v>
       </c>
-      <c r="E55" s="198"/>
+      <c r="E55" s="208"/>
       <c r="F55" s="152"/>
     </row>
     <row r="56" spans="2:6" ht="20" customHeight="1">
@@ -6901,10 +6907,10 @@
       <c r="C56" s="127" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="198" t="s">
+      <c r="D56" s="208" t="s">
         <v>128</v>
       </c>
-      <c r="E56" s="198"/>
+      <c r="E56" s="208"/>
       <c r="F56" s="152"/>
     </row>
     <row r="59" spans="2:6">
@@ -6920,10 +6926,10 @@
       <c r="C60" s="150" t="s">
         <v>350</v>
       </c>
-      <c r="D60" s="199" t="s">
+      <c r="D60" s="209" t="s">
         <v>354</v>
       </c>
-      <c r="E60" s="199"/>
+      <c r="E60" s="209"/>
       <c r="F60" s="150" t="s">
         <v>351</v>
       </c>
@@ -6935,10 +6941,10 @@
       <c r="C61" s="127" t="s">
         <v>130</v>
       </c>
-      <c r="D61" s="200" t="s">
+      <c r="D61" s="210" t="s">
         <v>135</v>
       </c>
-      <c r="E61" s="201"/>
+      <c r="E61" s="211"/>
       <c r="F61" s="152"/>
     </row>
     <row r="62" spans="2:6" ht="15" customHeight="1">
@@ -6948,10 +6954,10 @@
       <c r="C62" s="127" t="s">
         <v>131</v>
       </c>
-      <c r="D62" s="200" t="s">
+      <c r="D62" s="210" t="s">
         <v>136</v>
       </c>
-      <c r="E62" s="201"/>
+      <c r="E62" s="211"/>
       <c r="F62" s="152"/>
     </row>
     <row r="63" spans="2:6" ht="15" customHeight="1">
@@ -6961,10 +6967,10 @@
       <c r="C63" s="127" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="200" t="s">
+      <c r="D63" s="210" t="s">
         <v>137</v>
       </c>
-      <c r="E63" s="201"/>
+      <c r="E63" s="211"/>
       <c r="F63" s="152"/>
     </row>
     <row r="64" spans="2:6" ht="15" customHeight="1">
@@ -6974,10 +6980,10 @@
       <c r="C64" s="127" t="s">
         <v>133</v>
       </c>
-      <c r="D64" s="200" t="s">
+      <c r="D64" s="210" t="s">
         <v>138</v>
       </c>
-      <c r="E64" s="201"/>
+      <c r="E64" s="211"/>
       <c r="F64" s="152"/>
     </row>
     <row r="65" spans="2:6">
@@ -6987,29 +6993,21 @@
       <c r="C65" s="127" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="200"/>
-      <c r="E65" s="201"/>
+      <c r="D65" s="210"/>
+      <c r="E65" s="211"/>
       <c r="F65" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="D23:E23"/>
@@ -7026,19 +7024,27 @@
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7055,7 +7061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -7119,10 +7125,10 @@
       <c r="D4" s="104" t="s">
         <v>230</v>
       </c>
-      <c r="E4" s="202" t="s">
+      <c r="E4" s="213" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="203"/>
+      <c r="F4" s="214"/>
       <c r="G4" s="104" t="s">
         <v>211</v>
       </c>
@@ -7137,7 +7143,7 @@
       <c r="C5" s="106" t="s">
         <v>231</v>
       </c>
-      <c r="D5" s="204" t="s">
+      <c r="D5" s="215" t="s">
         <v>203</v>
       </c>
       <c r="E5" s="107" t="s">
@@ -7162,7 +7168,7 @@
       <c r="C6" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="205"/>
+      <c r="D6" s="216"/>
       <c r="E6" s="107" t="s">
         <v>206</v>
       </c>
@@ -7185,7 +7191,7 @@
       <c r="C7" s="106" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="205"/>
+      <c r="D7" s="216"/>
       <c r="E7" s="107" t="s">
         <v>207</v>
       </c>
@@ -7208,7 +7214,7 @@
       <c r="C8" s="106" t="s">
         <v>336</v>
       </c>
-      <c r="D8" s="205"/>
+      <c r="D8" s="216"/>
       <c r="E8" s="137" t="s">
         <v>207</v>
       </c>
@@ -7231,7 +7237,7 @@
       <c r="C9" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="D9" s="205"/>
+      <c r="D9" s="216"/>
       <c r="E9" s="107" t="s">
         <v>209</v>
       </c>
@@ -7254,7 +7260,7 @@
       <c r="C10" s="106" t="s">
         <v>328</v>
       </c>
-      <c r="D10" s="205"/>
+      <c r="D10" s="216"/>
       <c r="E10" s="137" t="s">
         <v>209</v>
       </c>
@@ -7279,7 +7285,7 @@
       <c r="C11" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="D11" s="206"/>
+      <c r="D11" s="217"/>
       <c r="E11" s="107" t="s">
         <v>207</v>
       </c>
@@ -7302,7 +7308,7 @@
       <c r="C12" s="111" t="s">
         <v>239</v>
       </c>
-      <c r="D12" s="207" t="s">
+      <c r="D12" s="218" t="s">
         <v>204</v>
       </c>
       <c r="E12" s="112" t="s">
@@ -7327,7 +7333,7 @@
       <c r="C13" s="111" t="s">
         <v>337</v>
       </c>
-      <c r="D13" s="208"/>
+      <c r="D13" s="219"/>
       <c r="E13" s="140" t="s">
         <v>209</v>
       </c>
@@ -7352,7 +7358,7 @@
       <c r="C14" s="111" t="s">
         <v>237</v>
       </c>
-      <c r="D14" s="208"/>
+      <c r="D14" s="219"/>
       <c r="E14" s="112" t="s">
         <v>209</v>
       </c>
@@ -7375,7 +7381,7 @@
       <c r="C15" s="111" t="s">
         <v>236</v>
       </c>
-      <c r="D15" s="208"/>
+      <c r="D15" s="219"/>
       <c r="E15" s="112" t="s">
         <v>209</v>
       </c>
@@ -7398,7 +7404,7 @@
       <c r="C16" s="111" t="s">
         <v>249</v>
       </c>
-      <c r="D16" s="208"/>
+      <c r="D16" s="219"/>
       <c r="E16" s="112" t="s">
         <v>209</v>
       </c>
@@ -7421,7 +7427,7 @@
       <c r="C17" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="208"/>
+      <c r="D17" s="219"/>
       <c r="E17" s="112" t="s">
         <v>206</v>
       </c>
@@ -7444,7 +7450,7 @@
       <c r="C18" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="D18" s="208"/>
+      <c r="D18" s="219"/>
       <c r="E18" s="112" t="s">
         <v>207</v>
       </c>
@@ -7467,7 +7473,7 @@
       <c r="C19" s="111" t="s">
         <v>242</v>
       </c>
-      <c r="D19" s="208"/>
+      <c r="D19" s="219"/>
       <c r="E19" s="112" t="s">
         <v>208</v>
       </c>
@@ -7490,7 +7496,7 @@
       <c r="C20" s="115" t="s">
         <v>243</v>
       </c>
-      <c r="D20" s="209" t="s">
+      <c r="D20" s="220" t="s">
         <v>205</v>
       </c>
       <c r="E20" s="116" t="s">
@@ -7515,7 +7521,7 @@
       <c r="C21" s="115" t="s">
         <v>244</v>
       </c>
-      <c r="D21" s="210"/>
+      <c r="D21" s="221"/>
       <c r="E21" s="116" t="s">
         <v>209</v>
       </c>
@@ -7538,7 +7544,7 @@
       <c r="C22" s="115" t="s">
         <v>245</v>
       </c>
-      <c r="D22" s="210"/>
+      <c r="D22" s="221"/>
       <c r="E22" s="116" t="s">
         <v>209</v>
       </c>
@@ -7561,7 +7567,7 @@
       <c r="C23" s="115" t="s">
         <v>246</v>
       </c>
-      <c r="D23" s="210"/>
+      <c r="D23" s="221"/>
       <c r="E23" s="116" t="s">
         <v>206</v>
       </c>
@@ -7584,7 +7590,7 @@
       <c r="C24" s="115" t="s">
         <v>247</v>
       </c>
-      <c r="D24" s="210"/>
+      <c r="D24" s="221"/>
       <c r="E24" s="116" t="s">
         <v>207</v>
       </c>
@@ -7607,7 +7613,7 @@
       <c r="C25" s="115" t="s">
         <v>248</v>
       </c>
-      <c r="D25" s="211"/>
+      <c r="D25" s="222"/>
       <c r="E25" s="116" t="s">
         <v>208</v>
       </c>
@@ -7727,6 +7733,7 @@
     <mergeCell ref="D12:D19"/>
     <mergeCell ref="D20:D25"/>
   </mergeCells>
+  <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -7741,8 +7748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -7783,7 +7790,7 @@
       <c r="A2" s="68" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="240" t="s">
+      <c r="B2" s="162" t="s">
         <v>367</v>
       </c>
       <c r="C2" s="66"/>
@@ -7824,15 +7831,15 @@
       <c r="B4" s="70" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="212" t="s">
+      <c r="C4" s="223" t="s">
         <v>231</v>
       </c>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
-      <c r="I4" s="213"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="231"/>
+      <c r="H4" s="231"/>
+      <c r="I4" s="224"/>
       <c r="J4" s="66"/>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
@@ -7845,15 +7852,15 @@
       <c r="B5" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="C5" s="212" t="s">
+      <c r="C5" s="223" t="s">
         <v>217</v>
       </c>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="222"/>
-      <c r="G5" s="222"/>
-      <c r="H5" s="222"/>
-      <c r="I5" s="213"/>
+      <c r="D5" s="231"/>
+      <c r="E5" s="231"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="231"/>
+      <c r="H5" s="231"/>
+      <c r="I5" s="224"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
@@ -7887,15 +7894,15 @@
       <c r="B7" s="70" t="s">
         <v>289</v>
       </c>
-      <c r="C7" s="212" t="s">
+      <c r="C7" s="223" t="s">
         <v>206</v>
       </c>
-      <c r="D7" s="222"/>
-      <c r="E7" s="222"/>
-      <c r="F7" s="222"/>
-      <c r="G7" s="222"/>
-      <c r="H7" s="222"/>
-      <c r="I7" s="213"/>
+      <c r="D7" s="231"/>
+      <c r="E7" s="231"/>
+      <c r="F7" s="231"/>
+      <c r="G7" s="231"/>
+      <c r="H7" s="231"/>
+      <c r="I7" s="224"/>
       <c r="J7" s="66"/>
       <c r="K7" s="66"/>
       <c r="L7" s="66"/>
@@ -7929,15 +7936,15 @@
       <c r="B9" s="70" t="s">
         <v>323</v>
       </c>
-      <c r="C9" s="212" t="s">
+      <c r="C9" s="223" t="s">
         <v>324</v>
       </c>
-      <c r="D9" s="222"/>
-      <c r="E9" s="222"/>
-      <c r="F9" s="222"/>
-      <c r="G9" s="222"/>
-      <c r="H9" s="222"/>
-      <c r="I9" s="213"/>
+      <c r="D9" s="231"/>
+      <c r="E9" s="231"/>
+      <c r="F9" s="231"/>
+      <c r="G9" s="231"/>
+      <c r="H9" s="231"/>
+      <c r="I9" s="224"/>
       <c r="J9" s="66"/>
       <c r="K9" s="66"/>
       <c r="L9" s="66"/>
@@ -8000,19 +8007,19 @@
     </row>
     <row r="13" spans="1:15" ht="20" customHeight="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="219" t="s">
+      <c r="B13" s="225" t="s">
         <v>165</v>
       </c>
-      <c r="C13" s="220"/>
-      <c r="D13" s="220"/>
-      <c r="E13" s="220"/>
-      <c r="F13" s="220"/>
-      <c r="G13" s="220"/>
-      <c r="H13" s="220"/>
-      <c r="I13" s="220"/>
-      <c r="J13" s="220"/>
-      <c r="K13" s="220"/>
-      <c r="L13" s="221"/>
+      <c r="C13" s="226"/>
+      <c r="D13" s="226"/>
+      <c r="E13" s="226"/>
+      <c r="F13" s="226"/>
+      <c r="G13" s="226"/>
+      <c r="H13" s="226"/>
+      <c r="I13" s="226"/>
+      <c r="J13" s="226"/>
+      <c r="K13" s="226"/>
+      <c r="L13" s="227"/>
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
       <c r="O13" s="66"/>
@@ -8041,11 +8048,11 @@
       <c r="I14" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="J14" s="223" t="s">
+      <c r="J14" s="232" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="223"/>
-      <c r="L14" s="223"/>
+      <c r="K14" s="232"/>
+      <c r="L14" s="232"/>
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
       <c r="O14" s="66"/>
@@ -8074,11 +8081,11 @@
       <c r="I15" s="81" t="s">
         <v>282</v>
       </c>
-      <c r="J15" s="224" t="s">
+      <c r="J15" s="233" t="s">
         <v>283</v>
       </c>
-      <c r="K15" s="224"/>
-      <c r="L15" s="224"/>
+      <c r="K15" s="233"/>
+      <c r="L15" s="233"/>
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
@@ -8107,11 +8114,11 @@
       <c r="I16" s="81" t="s">
         <v>286</v>
       </c>
-      <c r="J16" s="224" t="s">
+      <c r="J16" s="233" t="s">
         <v>287</v>
       </c>
-      <c r="K16" s="224"/>
-      <c r="L16" s="224"/>
+      <c r="K16" s="233"/>
+      <c r="L16" s="233"/>
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
@@ -8173,11 +8180,11 @@
       <c r="I18" s="79" t="s">
         <v>295</v>
       </c>
-      <c r="J18" s="212" t="s">
+      <c r="J18" s="223" t="s">
         <v>298</v>
       </c>
-      <c r="K18" s="222"/>
-      <c r="L18" s="213"/>
+      <c r="K18" s="231"/>
+      <c r="L18" s="224"/>
       <c r="M18" s="66"/>
       <c r="N18" s="66"/>
       <c r="O18" s="66"/>
@@ -8206,11 +8213,11 @@
       <c r="I19" s="83" t="s">
         <v>302</v>
       </c>
-      <c r="J19" s="212" t="s">
+      <c r="J19" s="223" t="s">
         <v>303</v>
       </c>
-      <c r="K19" s="222"/>
-      <c r="L19" s="213"/>
+      <c r="K19" s="231"/>
+      <c r="L19" s="224"/>
       <c r="M19" s="66"/>
       <c r="N19" s="66"/>
       <c r="O19" s="66"/>
@@ -8372,11 +8379,11 @@
     </row>
     <row r="29" spans="1:15" s="89" customFormat="1" ht="20" customHeight="1">
       <c r="A29" s="69"/>
-      <c r="B29" s="225" t="s">
+      <c r="B29" s="234" t="s">
         <v>291</v>
       </c>
-      <c r="C29" s="225"/>
-      <c r="D29" s="225"/>
+      <c r="C29" s="234"/>
+      <c r="D29" s="234"/>
       <c r="E29" s="87"/>
       <c r="F29" s="88"/>
       <c r="G29" s="87"/>
@@ -8391,12 +8398,12 @@
     </row>
     <row r="30" spans="1:15" s="91" customFormat="1" ht="20" customHeight="1">
       <c r="A30" s="90"/>
-      <c r="B30" s="216" t="s">
+      <c r="B30" s="228" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="217"/>
-      <c r="D30" s="217"/>
-      <c r="E30" s="218"/>
+      <c r="C30" s="229"/>
+      <c r="D30" s="229"/>
+      <c r="E30" s="230"/>
       <c r="F30" s="76" t="s">
         <v>166</v>
       </c>
@@ -8488,10 +8495,10 @@
       <c r="A33" s="66"/>
       <c r="B33" s="92"/>
       <c r="C33" s="97"/>
-      <c r="D33" s="212" t="s">
+      <c r="D33" s="223" t="s">
         <v>309</v>
       </c>
-      <c r="E33" s="213"/>
+      <c r="E33" s="224"/>
       <c r="F33" s="78" t="s">
         <v>182</v>
       </c>
@@ -8521,10 +8528,10 @@
       <c r="A34" s="66"/>
       <c r="B34" s="92"/>
       <c r="C34" s="99"/>
-      <c r="D34" s="212" t="s">
+      <c r="D34" s="223" t="s">
         <v>310</v>
       </c>
-      <c r="E34" s="213"/>
+      <c r="E34" s="224"/>
       <c r="F34" s="78" t="s">
         <v>311</v>
       </c>
@@ -8587,10 +8594,10 @@
       <c r="A36" s="66"/>
       <c r="B36" s="92"/>
       <c r="C36" s="102"/>
-      <c r="D36" s="212" t="s">
+      <c r="D36" s="223" t="s">
         <v>313</v>
       </c>
-      <c r="E36" s="213"/>
+      <c r="E36" s="224"/>
       <c r="F36" s="78" t="s">
         <v>315</v>
       </c>
@@ -8620,10 +8627,10 @@
       <c r="A37" s="66"/>
       <c r="B37" s="92"/>
       <c r="C37" s="102"/>
-      <c r="D37" s="214" t="s">
+      <c r="D37" s="237" t="s">
         <v>279</v>
       </c>
-      <c r="E37" s="215"/>
+      <c r="E37" s="238"/>
       <c r="F37" s="78" t="s">
         <v>280</v>
       </c>
@@ -8653,10 +8660,10 @@
       <c r="A38" s="66"/>
       <c r="B38" s="92"/>
       <c r="C38" s="97"/>
-      <c r="D38" s="212" t="s">
+      <c r="D38" s="223" t="s">
         <v>299</v>
       </c>
-      <c r="E38" s="213"/>
+      <c r="E38" s="224"/>
       <c r="F38" s="78" t="s">
         <v>292</v>
       </c>
@@ -8723,7 +8730,7 @@
         <v>300</v>
       </c>
       <c r="E40" s="151"/>
-      <c r="F40" s="232" t="s">
+      <c r="F40" s="157" t="s">
         <v>301</v>
       </c>
       <c r="G40" s="80" t="s">
@@ -8741,7 +8748,7 @@
       <c r="K40" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="L40" s="234" t="s">
+      <c r="L40" s="159" t="s">
         <v>366</v>
       </c>
       <c r="M40" s="66"/>
@@ -8752,10 +8759,10 @@
       <c r="A41" s="66"/>
       <c r="B41" s="98"/>
       <c r="C41" s="99"/>
-      <c r="D41" s="212" t="s">
+      <c r="D41" s="223" t="s">
         <v>183</v>
       </c>
-      <c r="E41" s="213"/>
+      <c r="E41" s="224"/>
       <c r="F41" s="78" t="s">
         <v>184</v>
       </c>
@@ -9091,11 +9098,11 @@
     </row>
     <row r="60" spans="1:15" ht="20" customHeight="1">
       <c r="A60" s="66"/>
-      <c r="B60" s="226" t="s">
+      <c r="B60" s="235" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="226"/>
-      <c r="D60" s="226"/>
+      <c r="C60" s="235"/>
+      <c r="D60" s="235"/>
       <c r="E60" s="66"/>
       <c r="F60" s="66"/>
       <c r="G60" s="66"/>
@@ -9112,12 +9119,12 @@
     </row>
     <row r="61" spans="1:15" s="91" customFormat="1" ht="20" customHeight="1">
       <c r="A61" s="90"/>
-      <c r="B61" s="216" t="s">
+      <c r="B61" s="228" t="s">
         <v>167</v>
       </c>
-      <c r="C61" s="217"/>
-      <c r="D61" s="217"/>
-      <c r="E61" s="218"/>
+      <c r="C61" s="229"/>
+      <c r="D61" s="229"/>
+      <c r="E61" s="230"/>
       <c r="F61" s="76" t="s">
         <v>166</v>
       </c>
@@ -9209,10 +9216,10 @@
       <c r="A64" s="66"/>
       <c r="B64" s="92"/>
       <c r="C64" s="97"/>
-      <c r="D64" s="235" t="s">
+      <c r="D64" s="236" t="s">
         <v>309</v>
       </c>
-      <c r="E64" s="213"/>
+      <c r="E64" s="224"/>
       <c r="F64" s="78" t="s">
         <v>182</v>
       </c>
@@ -9231,7 +9238,7 @@
       <c r="K64" s="80" t="s">
         <v>187</v>
       </c>
-      <c r="L64" s="234" t="s">
+      <c r="L64" s="159" t="s">
         <v>359</v>
       </c>
       <c r="M64" s="66"/>
@@ -9242,14 +9249,14 @@
       <c r="A65" s="66"/>
       <c r="B65" s="92"/>
       <c r="C65" s="97"/>
-      <c r="D65" s="235" t="s">
+      <c r="D65" s="236" t="s">
         <v>0</v>
       </c>
-      <c r="E65" s="236"/>
-      <c r="F65" s="232" t="s">
+      <c r="E65" s="239"/>
+      <c r="F65" s="157" t="s">
         <v>357</v>
       </c>
-      <c r="G65" s="233" t="s">
+      <c r="G65" s="158" t="s">
         <v>281</v>
       </c>
       <c r="H65" s="80" t="s">
@@ -9258,13 +9265,13 @@
       <c r="I65" s="80">
         <v>1</v>
       </c>
-      <c r="J65" s="233" t="s">
+      <c r="J65" s="158" t="s">
         <v>174</v>
       </c>
-      <c r="K65" s="233" t="s">
+      <c r="K65" s="158" t="s">
         <v>174</v>
       </c>
-      <c r="L65" s="234" t="s">
+      <c r="L65" s="159" t="s">
         <v>358</v>
       </c>
       <c r="M65" s="66"/>
@@ -9275,11 +9282,11 @@
       <c r="A66" s="66"/>
       <c r="B66" s="92"/>
       <c r="C66" s="97"/>
-      <c r="D66" s="238" t="s">
+      <c r="D66" s="240" t="s">
         <v>362</v>
       </c>
-      <c r="E66" s="236"/>
-      <c r="F66" s="232" t="s">
+      <c r="E66" s="239"/>
+      <c r="F66" s="157" t="s">
         <v>360</v>
       </c>
       <c r="G66" s="80" t="s">
@@ -9297,7 +9304,7 @@
       <c r="K66" s="80" t="s">
         <v>187</v>
       </c>
-      <c r="L66" s="234" t="s">
+      <c r="L66" s="159" t="s">
         <v>365</v>
       </c>
       <c r="M66" s="66"/>
@@ -9308,29 +9315,29 @@
       <c r="A67" s="66"/>
       <c r="B67" s="92"/>
       <c r="C67" s="102"/>
-      <c r="D67" s="239"/>
-      <c r="E67" s="237" t="s">
+      <c r="D67" s="161"/>
+      <c r="E67" s="160" t="s">
         <v>363</v>
       </c>
-      <c r="F67" s="232" t="s">
+      <c r="F67" s="157" t="s">
         <v>311</v>
       </c>
-      <c r="G67" s="233" t="s">
+      <c r="G67" s="158" t="s">
         <v>281</v>
       </c>
       <c r="H67" s="80" t="s">
         <v>304</v>
       </c>
-      <c r="I67" s="233" t="s">
+      <c r="I67" s="158" t="s">
         <v>361</v>
       </c>
-      <c r="J67" s="233" t="s">
+      <c r="J67" s="158" t="s">
         <v>174</v>
       </c>
-      <c r="K67" s="233" t="s">
+      <c r="K67" s="158" t="s">
         <v>174</v>
       </c>
-      <c r="L67" s="234" t="s">
+      <c r="L67" s="159" t="s">
         <v>364</v>
       </c>
       <c r="M67" s="66"/>
@@ -9372,8 +9379,8 @@
       <c r="A69" s="66"/>
       <c r="B69" s="98"/>
       <c r="C69" s="99"/>
-      <c r="D69" s="212"/>
-      <c r="E69" s="213"/>
+      <c r="D69" s="223"/>
+      <c r="E69" s="224"/>
       <c r="F69" s="78"/>
       <c r="G69" s="80"/>
       <c r="H69" s="80"/>
@@ -9763,6 +9770,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B61:E61"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B30:E30"/>
@@ -9779,14 +9794,6 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <hyperlinks>

</xml_diff>